<commit_message>
Technical event students participation data added from MGM Curry sheet
</commit_message>
<xml_diff>
--- a/C2/C2 NBA All Tables Conso.xlsx
+++ b/C2/C2 NBA All Tables Conso.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="317">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -1011,7 +1011,28 @@
     <t>Format : List of Students Participated in Technical events at national/state/inter institute level</t>
   </si>
   <si>
-    <t>This data is collected from Certificates Received from MGM in Yellow File</t>
+    <t>Jadhav Madhuri G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poster Presentation </t>
+  </si>
+  <si>
+    <t>MindLabz Pvt. Ltd. Latur</t>
+  </si>
+  <si>
+    <t>1/2/2018- 2/2/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participation </t>
+  </si>
+  <si>
+    <t>Bade Vaishanvi D</t>
+  </si>
+  <si>
+    <t>Deshmane Summaiya S</t>
+  </si>
+  <si>
+    <t>This data is collected from Certificates Received from MGM in Yellow File as well as monitoring sheets</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1042,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1123,6 +1144,13 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1360,7 +1388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1466,14 +1494,17 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1511,12 +1542,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1532,14 +1557,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1813,7 +1844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1836,21 +1867,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="2" t="s">
@@ -1868,11 +1899,11 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
     </row>
     <row r="5" spans="2:12" ht="22.5">
       <c r="B5" s="6">
@@ -1988,8 +2019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L89"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2005,39 +2036,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="19.5" customHeight="1">
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="H2" s="40" t="s">
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="H2" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="51"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
-      <c r="J5" s="41" t="s">
+      <c r="J5" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="44"/>
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="10" t="s">
@@ -2061,9 +2092,9 @@
       <c r="H6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="44"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="46"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="47"/>
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="4">
@@ -2085,9 +2116,9 @@
         <v>39</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="46"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="47"/>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="4">
@@ -2109,9 +2140,9 @@
         <v>39</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="46"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="47"/>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="4">
@@ -2133,9 +2164,9 @@
         <v>39</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="49"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="50"/>
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="4">
@@ -2387,10 +2418,10 @@
       <c r="H22" s="17"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="51"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
@@ -2967,10 +2998,10 @@
       <c r="H51" s="4"/>
     </row>
     <row r="54" spans="2:8" ht="16.5" thickBot="1">
-      <c r="B54" s="52" t="s">
+      <c r="B54" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="52"/>
+      <c r="C54" s="39"/>
     </row>
     <row r="55" spans="2:8">
       <c r="B55" s="22" t="s">
@@ -3206,10 +3237,10 @@
       <c r="H65" s="9"/>
     </row>
     <row r="69" spans="2:8" ht="15.75">
-      <c r="B69" s="52" t="s">
+      <c r="B69" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="C69" s="53"/>
+      <c r="C69" s="40"/>
     </row>
     <row r="70" spans="2:8">
       <c r="B70" s="22" t="s">
@@ -3652,7 +3683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -3667,13 +3698,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5">
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" customHeight="1">
       <c r="B2" s="12"/>
@@ -3681,43 +3712,43 @@
       <c r="D2" s="27"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="44"/>
     </row>
     <row r="3" spans="1:15" ht="15.75">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="49"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="50"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
     </row>
     <row r="6" spans="1:15" ht="51.75" customHeight="1">
       <c r="A6" s="10" t="s">
@@ -4048,14 +4079,14 @@
       <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
     </row>
     <row r="24" spans="1:6" ht="51">
       <c r="A24" s="10" t="s">
@@ -4314,14 +4345,14 @@
       <c r="F37" s="33"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="56"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="55"/>
     </row>
     <row r="39" spans="1:6" ht="38.25">
       <c r="A39" s="10" t="s">
@@ -4453,13 +4484,13 @@
     </row>
     <row r="46" spans="1:6" ht="24.95" customHeight="1">
       <c r="A46" s="2"/>
-      <c r="B46" s="54" t="s">
+      <c r="B46" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
     </row>
     <row r="47" spans="1:6" ht="38.25">
       <c r="A47" s="10" t="s">
@@ -4615,13 +4646,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="19.5">
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
     </row>
     <row r="3" spans="2:16" ht="19.5">
       <c r="C3" s="13"/>
@@ -4631,25 +4662,25 @@
       <c r="G3" s="13"/>
     </row>
     <row r="4" spans="2:16" ht="15.75">
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="58" t="s">
         <v>271</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
     </row>
     <row r="5" spans="2:16">
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="44"/>
     </row>
     <row r="6" spans="2:16">
       <c r="B6" s="59" t="s">
@@ -4657,14 +4688,14 @@
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="59"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="49"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="50"/>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" s="10" t="s">
@@ -5494,13 +5525,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B52:D52"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="I5:P6"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B52:D52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5509,30 +5540,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:O34"/>
+  <dimension ref="C2:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
-    <col min="5" max="5" width="61.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" customWidth="1"/>
+    <col min="5" max="5" width="80.5703125" customWidth="1"/>
     <col min="6" max="6" width="28.28515625" customWidth="1"/>
     <col min="7" max="7" width="46.5703125" customWidth="1"/>
-    <col min="8" max="8" width="28.42578125" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:15" ht="19.5">
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
     </row>
     <row r="3" spans="3:15" ht="19.5">
       <c r="D3" s="13"/>
@@ -5540,45 +5571,45 @@
       <c r="F3" s="27"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="J3" s="61" t="s">
-        <v>309</v>
-      </c>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
+      <c r="J3" s="60" t="s">
+        <v>316</v>
+      </c>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
     </row>
     <row r="4" spans="3:15" ht="15.75">
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="58" t="s">
         <v>308</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
     </row>
     <row r="5" spans="3:15">
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
     </row>
     <row r="6" spans="3:15">
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="61"/>
-      <c r="N6" s="61"/>
-      <c r="O6" s="61"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
     </row>
     <row r="7" spans="3:15">
       <c r="C7" s="59" t="s">
@@ -5632,7 +5663,7 @@
       <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="4" t="s">
         <v>280</v>
       </c>
       <c r="E10" s="9" t="s">
@@ -5652,7 +5683,7 @@
       <c r="C11" s="9">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="4" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="9" t="s">
@@ -5672,7 +5703,7 @@
       <c r="C12" s="1">
         <v>4</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="4" t="s">
         <v>282</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -5692,19 +5723,19 @@
       <c r="C13" s="9">
         <v>5</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="4" t="s">
         <v>287</v>
       </c>
     </row>
@@ -5712,19 +5743,19 @@
       <c r="C14" s="1">
         <v>6</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="4" t="s">
         <v>287</v>
       </c>
     </row>
@@ -5732,19 +5763,19 @@
       <c r="C15" s="9">
         <v>7</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="62">
         <v>43831</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="4" t="s">
         <v>291</v>
       </c>
     </row>
@@ -5752,143 +5783,173 @@
       <c r="C16" s="1">
         <v>8</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="F16" s="37">
+      <c r="F16" s="62">
         <v>43831</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="4" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="17" spans="3:8">
+    <row r="17" spans="3:16">
       <c r="C17" s="9">
         <v>9</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="F17" s="37">
+      <c r="F17" s="62">
         <v>43831</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="4" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="3:8" ht="30">
+    <row r="18" spans="3:16" ht="15" customHeight="1">
       <c r="C18" s="1">
         <v>10</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="19" spans="3:8" ht="30">
+    <row r="19" spans="3:16" ht="18" customHeight="1">
       <c r="C19" s="9">
         <v>11</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="20" spans="3:8">
+    <row r="20" spans="3:16">
       <c r="C20" s="1">
         <v>12</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="F20" s="35">
+      <c r="F20" s="30">
         <v>43352</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="4" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="21" spans="3:8">
+    <row r="21" spans="3:16">
       <c r="C21" s="9">
         <v>13</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="3:8">
+      <c r="D21" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="22" spans="3:16">
       <c r="C22" s="1">
         <v>14</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="3:8">
+      <c r="D22" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16">
       <c r="C23" s="9">
         <v>15</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="3:8">
+      <c r="D23" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="3:16">
       <c r="C24" s="1">
         <v>16</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="3:8">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="3:16">
       <c r="C25" s="9">
         <v>17</v>
       </c>
@@ -5898,7 +5959,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="3:8">
+    <row r="26" spans="3:16">
       <c r="C26" s="1">
         <v>18</v>
       </c>
@@ -5908,7 +5969,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="3:8">
+    <row r="27" spans="3:16" ht="15.75">
       <c r="C27" s="9">
         <v>19</v>
       </c>
@@ -5917,8 +5978,11 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="3:8">
+      <c r="L27" s="61"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="61"/>
+    </row>
+    <row r="28" spans="3:16" ht="15.75">
       <c r="C28" s="1">
         <v>20</v>
       </c>
@@ -5927,8 +5991,11 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="3:8">
+      <c r="L28" s="61"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="61"/>
+    </row>
+    <row r="29" spans="3:16" ht="15.75">
       <c r="C29" s="9">
         <v>21</v>
       </c>
@@ -5937,8 +6004,11 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="3:8">
+      <c r="L29" s="61"/>
+      <c r="O29" s="61"/>
+      <c r="P29" s="61"/>
+    </row>
+    <row r="30" spans="3:16">
       <c r="C30" s="1">
         <v>22</v>
       </c>
@@ -5948,7 +6018,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="3:8">
+    <row r="31" spans="3:16">
       <c r="C31" s="9">
         <v>23</v>
       </c>
@@ -5958,7 +6028,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="3:8">
+    <row r="32" spans="3:16">
       <c r="C32" s="1">
         <v>24</v>
       </c>
@@ -5996,5 +6066,6 @@
     <mergeCell ref="D4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tech Event from MGM Yellow file AM 2018 19 added
</commit_message>
<xml_diff>
--- a/C2/C2 NBA All Tables Conso.xlsx
+++ b/C2/C2 NBA All Tables Conso.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="323">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -1033,6 +1033,24 @@
   </si>
   <si>
     <t>This data is collected from Certificates Received from MGM in Yellow File as well as monitoring sheets</t>
+  </si>
+  <si>
+    <t>Tandale Harshita</t>
+  </si>
+  <si>
+    <t>Workshop on Career Plan</t>
+  </si>
+  <si>
+    <t>Seed Infotech Pune</t>
+  </si>
+  <si>
+    <t>Swami Jyoti</t>
+  </si>
+  <si>
+    <t>C and C++ Code competition</t>
+  </si>
+  <si>
+    <t>BIT College Barshi</t>
   </si>
 </sst>
 </file>
@@ -1494,6 +1512,12 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1557,20 +1581,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1844,7 +1862,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1867,21 +1885,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="2" t="s">
@@ -1899,11 +1917,11 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
     </row>
     <row r="5" spans="2:12" ht="22.5">
       <c r="B5" s="6">
@@ -2036,39 +2054,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="19.5" customHeight="1">
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="H2" s="41" t="s">
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="H2" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="52"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="K5" s="43"/>
-      <c r="L5" s="44"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="46"/>
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="10" t="s">
@@ -2092,9 +2110,9 @@
       <c r="H6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="45"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="49"/>
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="4">
@@ -2116,9 +2134,9 @@
         <v>39</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="49"/>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="4">
@@ -2140,9 +2158,9 @@
         <v>39</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="49"/>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="4">
@@ -2164,9 +2182,9 @@
         <v>39</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="52"/>
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="4">
@@ -2418,10 +2436,10 @@
       <c r="H22" s="17"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="52"/>
+      <c r="C24" s="54"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
@@ -2998,10 +3016,10 @@
       <c r="H51" s="4"/>
     </row>
     <row r="54" spans="2:8" ht="16.5" thickBot="1">
-      <c r="B54" s="39" t="s">
+      <c r="B54" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="39"/>
+      <c r="C54" s="41"/>
     </row>
     <row r="55" spans="2:8">
       <c r="B55" s="22" t="s">
@@ -3237,10 +3255,10 @@
       <c r="H65" s="9"/>
     </row>
     <row r="69" spans="2:8" ht="15.75">
-      <c r="B69" s="39" t="s">
+      <c r="B69" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="C69" s="40"/>
+      <c r="C69" s="42"/>
     </row>
     <row r="70" spans="2:8">
       <c r="B70" s="22" t="s">
@@ -3698,13 +3716,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" customHeight="1">
       <c r="B2" s="12"/>
@@ -3712,43 +3730,43 @@
       <c r="D2" s="27"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="44"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="46"/>
     </row>
     <row r="3" spans="1:15" ht="15.75">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="50"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="52"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
     </row>
     <row r="6" spans="1:15" ht="51.75" customHeight="1">
       <c r="A6" s="10" t="s">
@@ -4079,14 +4097,14 @@
       <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
     </row>
     <row r="24" spans="1:6" ht="51">
       <c r="A24" s="10" t="s">
@@ -4345,14 +4363,14 @@
       <c r="F37" s="33"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="55"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="57"/>
     </row>
     <row r="39" spans="1:6" ht="38.25">
       <c r="A39" s="10" t="s">
@@ -4484,13 +4502,13 @@
     </row>
     <row r="46" spans="1:6" ht="24.95" customHeight="1">
       <c r="A46" s="2"/>
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="C46" s="54"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="54"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
     </row>
     <row r="47" spans="1:6" ht="38.25">
       <c r="A47" s="10" t="s">
@@ -4646,13 +4664,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="19.5">
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
     </row>
     <row r="3" spans="2:16" ht="19.5">
       <c r="C3" s="13"/>
@@ -4662,40 +4680,40 @@
       <c r="G3" s="13"/>
     </row>
     <row r="4" spans="2:16" ht="15.75">
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="61" t="s">
         <v>271</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
     </row>
     <row r="5" spans="2:16">
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="44"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="46"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="50"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="52"/>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" s="10" t="s">
@@ -4894,11 +4912,11 @@
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="10" t="s">
@@ -5172,11 +5190,11 @@
       <c r="C33" s="34"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="59" t="s">
+      <c r="B36" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
     </row>
     <row r="37" spans="2:7">
       <c r="B37" s="10" t="s">
@@ -5427,11 +5445,11 @@
       <c r="G49" s="1"/>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="59" t="s">
+      <c r="B52" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="C52" s="59"/>
-      <c r="D52" s="59"/>
+      <c r="C52" s="60"/>
+      <c r="D52" s="60"/>
     </row>
     <row r="53" spans="2:7">
       <c r="B53" s="10" t="s">
@@ -5542,8 +5560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5557,13 +5575,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:15" ht="19.5">
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="3:15" ht="19.5">
       <c r="D3" s="13"/>
@@ -5571,53 +5589,53 @@
       <c r="F3" s="27"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="62" t="s">
         <v>316</v>
       </c>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
     </row>
     <row r="4" spans="3:15" ht="15.75">
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="61" t="s">
         <v>308</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
     </row>
     <row r="5" spans="3:15">
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
     </row>
     <row r="6" spans="3:15">
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
     </row>
     <row r="7" spans="3:15">
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
     </row>
     <row r="8" spans="3:15" ht="24" customHeight="1">
       <c r="C8" s="10" t="s">
@@ -5769,7 +5787,7 @@
       <c r="E15" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="F15" s="62">
+      <c r="F15" s="38">
         <v>43831</v>
       </c>
       <c r="G15" s="9" t="s">
@@ -5789,7 +5807,7 @@
       <c r="E16" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="F16" s="62">
+      <c r="F16" s="38">
         <v>43831</v>
       </c>
       <c r="G16" s="9" t="s">
@@ -5809,7 +5827,7 @@
       <c r="E17" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="F17" s="62">
+      <c r="F17" s="38">
         <v>43831</v>
       </c>
       <c r="G17" s="9" t="s">
@@ -5943,44 +5961,80 @@
       <c r="C24" s="1">
         <v>16</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="D24" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="F24" s="30">
+        <v>43352</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="25" spans="3:16">
       <c r="C25" s="9">
         <v>17</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>318</v>
+      </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="26" spans="3:16">
       <c r="C26" s="1">
         <v>18</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="27" spans="3:16" ht="15.75">
       <c r="C27" s="9">
         <v>19</v>
       </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>318</v>
+      </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="L27" s="61"/>
-      <c r="O27" s="61"/>
-      <c r="P27" s="61"/>
+      <c r="G27" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="L27" s="37"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
     </row>
     <row r="28" spans="3:16" ht="15.75">
       <c r="C28" s="1">
@@ -5991,9 +6045,9 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="L28" s="61"/>
-      <c r="O28" s="61"/>
-      <c r="P28" s="61"/>
+      <c r="L28" s="37"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="37"/>
     </row>
     <row r="29" spans="3:16" ht="15.75">
       <c r="C29" s="9">
@@ -6004,9 +6058,9 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="L29" s="61"/>
-      <c r="O29" s="61"/>
-      <c r="P29" s="61"/>
+      <c r="L29" s="37"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="37"/>
     </row>
     <row r="30" spans="3:16">
       <c r="C30" s="1">

</xml_diff>

<commit_message>
All yrs roll call from MGM and AM PPT added
</commit_message>
<xml_diff>
--- a/C2/C2 NBA All Tables Conso.xlsx
+++ b/C2/C2 NBA All Tables Conso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Personality develop. cell" sheetId="4" r:id="rId1"/>
@@ -1862,7 +1862,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2037,7 +2037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L89"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
@@ -3701,7 +3701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -4648,8 +4648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:P57"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5560,8 +5560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
16 17 Students participating institute name added in sheet Shree ramchandra college pf egg
</commit_message>
<xml_diff>
--- a/C2/C2 NBA All Tables Conso.xlsx
+++ b/C2/C2 NBA All Tables Conso.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Hostel Activities" sheetId="8" r:id="rId3"/>
     <sheet name="Activities Organised BY CO dept" sheetId="9" r:id="rId4"/>
     <sheet name="Students Participation in Techn" sheetId="10" r:id="rId5"/>
+    <sheet name="Sports Winner" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -354,9 +355,6 @@
     <t>Zonal Competition 2017 W-2 Zone</t>
   </si>
   <si>
-    <t>Pune</t>
-  </si>
-  <si>
     <t>2/2/2017 and 3/2/2017</t>
   </si>
   <si>
@@ -1048,6 +1046,9 @@
   </si>
   <si>
     <t>BIT College Barshi</t>
+  </si>
+  <si>
+    <t>Shree Ramchandra college of engineering,Pune</t>
   </si>
 </sst>
 </file>
@@ -1826,7 +1827,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1858,7 +1859,7 @@
     </row>
     <row r="3" spans="2:12">
       <c r="H3" s="38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I3" s="38"/>
       <c r="J3" s="38"/>
@@ -2001,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:G89"/>
+    <sheetView tabSelected="1" topLeftCell="B59" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2033,7 +2034,7 @@
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="I5" s="41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J5" s="42"/>
       <c r="K5" s="43"/>
@@ -2190,7 +2191,7 @@
         <v>38</v>
       </c>
       <c r="I12" s="40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J12" s="40"/>
       <c r="K12" s="40"/>
@@ -2932,7 +2933,7 @@
       </c>
       <c r="C54" s="39"/>
     </row>
-    <row r="55" spans="2:7">
+    <row r="55" spans="2:7" ht="25.5">
       <c r="B55" s="22" t="s">
         <v>28</v>
       </c>
@@ -2952,7 +2953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" spans="2:7" ht="25.5">
       <c r="B56" s="4">
         <v>1</v>
       </c>
@@ -2972,7 +2973,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" spans="2:7" ht="25.5">
       <c r="B57" s="4">
         <v>2</v>
       </c>
@@ -2992,7 +2993,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="2:7">
+    <row r="58" spans="2:7" ht="25.5">
       <c r="B58" s="4">
         <v>3</v>
       </c>
@@ -3012,7 +3013,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="2:7">
+    <row r="59" spans="2:7" ht="25.5">
       <c r="B59" s="4">
         <v>4</v>
       </c>
@@ -3032,7 +3033,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="2:7">
+    <row r="60" spans="2:7" ht="25.5">
       <c r="B60" s="4">
         <v>5</v>
       </c>
@@ -3179,7 +3180,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="2:7">
+    <row r="71" spans="2:7" ht="25.5">
       <c r="B71" s="4">
         <v>1</v>
       </c>
@@ -3193,58 +3194,58 @@
         <v>101</v>
       </c>
       <c r="F71" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G71" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="G71" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7">
+    </row>
+    <row r="72" spans="2:7" ht="25.5">
       <c r="B72" s="4">
         <v>2</v>
       </c>
       <c r="C72" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D72" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="E72" s="15" t="s">
         <v>101</v>
       </c>
       <c r="F72" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G72" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="G72" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7">
+    </row>
+    <row r="73" spans="2:7" ht="25.5">
       <c r="B73" s="4">
         <v>3</v>
       </c>
       <c r="C73" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D73" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="E73" s="15" t="s">
         <v>101</v>
       </c>
       <c r="F73" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G73" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="G73" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7">
+    </row>
+    <row r="74" spans="2:7" ht="25.5">
       <c r="B74" s="4">
         <v>4</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>48</v>
@@ -3253,18 +3254,18 @@
         <v>101</v>
       </c>
       <c r="F74" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G74" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="G74" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7">
+    </row>
+    <row r="75" spans="2:7" ht="25.5">
       <c r="B75" s="4">
         <v>5</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>48</v>
@@ -3273,50 +3274,50 @@
         <v>101</v>
       </c>
       <c r="F75" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G75" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="G75" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7">
+    </row>
+    <row r="76" spans="2:7" ht="25.5">
       <c r="B76" s="4">
         <v>6</v>
       </c>
       <c r="C76" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D76" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="E76" s="15" t="s">
         <v>101</v>
       </c>
       <c r="F76" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G76" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="G76" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="77" spans="2:7">
+    </row>
+    <row r="77" spans="2:7" ht="25.5">
       <c r="B77" s="4">
         <v>7</v>
       </c>
       <c r="C77" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D77" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="E77" s="15" t="s">
         <v>101</v>
       </c>
       <c r="F77" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G77" s="11" t="s">
         <v>102</v>
-      </c>
-      <c r="G77" s="11" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="78" spans="2:7">
@@ -3324,19 +3325,19 @@
         <v>8</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E78" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F78" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F78" s="4" t="s">
+      <c r="G78" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G78" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="79" spans="2:7">
@@ -3344,19 +3345,19 @@
         <v>9</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E79" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F79" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F79" s="4" t="s">
+      <c r="G79" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G79" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="80" spans="2:7">
@@ -3364,19 +3365,19 @@
         <v>10</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E80" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F80" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F80" s="4" t="s">
+      <c r="G80" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G80" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="81" spans="2:7">
@@ -3384,19 +3385,19 @@
         <v>11</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E81" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F81" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F81" s="4" t="s">
+      <c r="G81" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G81" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="82" spans="2:7">
@@ -3404,19 +3405,19 @@
         <v>12</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E82" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F82" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F82" s="4" t="s">
+      <c r="G82" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G82" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="83" spans="2:7">
@@ -3424,19 +3425,19 @@
         <v>13</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E83" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F83" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F83" s="4" t="s">
+      <c r="G83" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G83" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="84" spans="2:7">
@@ -3444,19 +3445,19 @@
         <v>14</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E84" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F84" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F84" s="4" t="s">
+      <c r="G84" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G84" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="85" spans="2:7">
@@ -3464,19 +3465,19 @@
         <v>15</v>
       </c>
       <c r="C85" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D85" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D85" s="9" t="s">
-        <v>125</v>
-      </c>
       <c r="E85" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F85" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="G85" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G85" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="86" spans="2:7">
@@ -3484,19 +3485,19 @@
         <v>16</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E86" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F86" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F86" s="4" t="s">
+      <c r="G86" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G86" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="87" spans="2:7">
@@ -3504,19 +3505,19 @@
         <v>17</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E87" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F87" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F87" s="4" t="s">
+      <c r="G87" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G87" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="88" spans="2:7">
@@ -3524,19 +3525,19 @@
         <v>18</v>
       </c>
       <c r="C88" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D88" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D88" s="9" t="s">
-        <v>129</v>
-      </c>
       <c r="E88" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F88" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F88" s="4" t="s">
+      <c r="G88" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G88" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="89" spans="2:7">
@@ -3544,30 +3545,30 @@
         <v>19</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E89" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F89" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F89" s="4" t="s">
+      <c r="G89" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G89" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B69:D69"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="I12:L13"/>
     <mergeCell ref="I5:K9"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B69:D69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3608,7 +3609,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="H2" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I2" s="42"/>
       <c r="J2" s="42"/>
@@ -3647,22 +3648,22 @@
     </row>
     <row r="6" spans="1:15" ht="51.75" customHeight="1">
       <c r="A6" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>134</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>135</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="38.25">
@@ -3670,19 +3671,19 @@
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C7" s="28">
         <v>43668</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7" s="4">
         <v>700</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="38.25">
@@ -3690,19 +3691,19 @@
         <v>2</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="28">
         <v>43686</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E8" s="4">
         <v>530</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="38.25">
@@ -3710,19 +3711,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C9" s="28">
         <v>43679</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E9" s="4">
         <v>600</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="38.25">
@@ -3730,19 +3731,19 @@
         <v>4</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" s="28">
         <v>44074</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E10" s="4">
         <v>600</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="37.5" customHeight="1">
@@ -3750,19 +3751,19 @@
         <v>5</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C11" s="28">
         <v>43729</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E11" s="4">
         <v>650</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="38.25" customHeight="1">
@@ -3770,19 +3771,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C12" s="28">
         <v>43776</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E12" s="4">
         <v>600</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="48.75" customHeight="1">
@@ -3790,19 +3791,19 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="E13" s="4">
         <v>130</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="32.25" customHeight="1">
@@ -3810,19 +3811,19 @@
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="E14" s="4">
         <v>600</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="30.75" customHeight="1">
@@ -3830,19 +3831,19 @@
         <v>9</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="E15" s="4">
         <v>600</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="38.25">
@@ -3850,19 +3851,19 @@
         <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" s="29">
         <v>43836</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E16" s="4">
         <v>600</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30.75" customHeight="1">
@@ -3870,19 +3871,19 @@
         <v>11</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C17" s="29">
         <v>43858</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E17" s="4">
         <v>700</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="63.75">
@@ -3890,19 +3891,19 @@
         <v>12</v>
       </c>
       <c r="B18" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="D18" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="E18" s="4">
         <v>100</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="38.25">
@@ -3910,19 +3911,19 @@
         <v>13</v>
       </c>
       <c r="B19" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>165</v>
-      </c>
       <c r="D19" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E19" s="4">
         <v>130</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="38.25">
@@ -3930,19 +3931,19 @@
         <v>14</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20" s="29">
         <v>43876</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E20" s="4">
         <v>270</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30.75" customHeight="1">
@@ -3950,19 +3951,19 @@
         <v>15</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C21" s="29">
         <v>43895</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E21" s="4">
         <v>500</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30.75" customHeight="1">
@@ -3985,22 +3986,22 @@
     </row>
     <row r="24" spans="1:6" ht="51">
       <c r="A24" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30.75" customHeight="1">
@@ -4008,19 +4009,19 @@
         <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C25" s="28">
         <v>43281</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E25" s="4">
         <v>250</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="25.5">
@@ -4028,19 +4029,19 @@
         <v>2</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C26" s="28">
         <v>43286</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E26" s="4">
         <v>200</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="38.25">
@@ -4048,19 +4049,19 @@
         <v>3</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C27" s="28">
         <v>43307</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E27" s="4">
         <v>285</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.5" customHeight="1">
@@ -4068,19 +4069,19 @@
         <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C28" s="28">
         <v>43321</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E28" s="4">
         <v>500</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="25.5">
@@ -4088,19 +4089,19 @@
         <v>5</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>175</v>
-      </c>
       <c r="D29" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E29" s="4">
         <v>650</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="31.5" customHeight="1">
@@ -4108,19 +4109,19 @@
         <v>6</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C30" s="28">
         <v>43332</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E30" s="4">
         <v>650</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="35.25" customHeight="1">
@@ -4128,19 +4129,19 @@
         <v>7</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C31" s="28">
         <v>43335</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E31" s="4">
         <v>600</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="33" customHeight="1">
@@ -4148,19 +4149,19 @@
         <v>8</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C32" s="28">
         <v>43349</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E32" s="4">
         <v>400</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="34.5" customHeight="1">
@@ -4168,19 +4169,19 @@
         <v>9</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C33" s="28">
         <v>43350</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E33" s="4">
         <v>400</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" customHeight="1">
@@ -4188,19 +4189,19 @@
         <v>10</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E34" s="4">
         <v>350</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="25.5">
@@ -4208,19 +4209,19 @@
         <v>11</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C35" s="28">
         <v>43472</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E35" s="4">
         <v>700</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -4251,22 +4252,22 @@
     </row>
     <row r="39" spans="1:6" ht="38.25">
       <c r="A39" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16.5" customHeight="1">
@@ -4274,19 +4275,19 @@
         <v>1</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C40" s="28">
         <v>42948</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E40" s="4">
         <v>250</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="16.5" customHeight="1">
@@ -4294,19 +4295,19 @@
         <v>2</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C41" s="28">
         <v>42967</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E41" s="4">
         <v>500</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="16.5" customHeight="1">
@@ -4314,19 +4315,19 @@
         <v>3</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C42" s="28">
         <v>43049</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E42" s="4">
         <v>600</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="16.5" customHeight="1">
@@ -4334,19 +4335,19 @@
         <v>4</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C43" s="28">
         <v>43105</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E43" s="4">
         <v>500</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="16.5" customHeight="1">
@@ -4354,19 +4355,19 @@
         <v>5</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C44" s="28">
         <v>43201</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E44" s="4">
         <v>600</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="24.95" customHeight="1">
@@ -4380,7 +4381,7 @@
     <row r="46" spans="1:6" ht="24.95" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C46" s="53"/>
       <c r="D46" s="53"/>
@@ -4389,22 +4390,22 @@
     </row>
     <row r="47" spans="1:6" ht="38.25">
       <c r="A47" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="16.5" customHeight="1">
@@ -4412,19 +4413,19 @@
         <v>1</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C48" s="28">
         <v>42585</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E48" s="4">
         <v>250</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="16.5" customHeight="1">
@@ -4432,19 +4433,19 @@
         <v>2</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C49" s="28">
         <v>42602</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E49" s="4">
         <v>500</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16.5" customHeight="1">
@@ -4452,19 +4453,19 @@
         <v>3</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C50" s="28">
         <v>42684</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E50" s="4">
         <v>600</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16.5" customHeight="1">
@@ -4472,19 +4473,19 @@
         <v>4</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C51" s="28">
         <v>42741</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E51" s="4">
         <v>500</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="16.5" customHeight="1">
@@ -4492,19 +4493,19 @@
         <v>5</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C52" s="28">
         <v>42826</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E52" s="4">
         <v>600</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -4558,7 +4559,7 @@
     </row>
     <row r="4" spans="2:16" ht="15.75">
       <c r="C4" s="58" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D4" s="58"/>
       <c r="E4" s="58"/>
@@ -4567,7 +4568,7 @@
     </row>
     <row r="5" spans="2:16">
       <c r="I5" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J5" s="42"/>
       <c r="K5" s="42"/>
@@ -4597,13 +4598,13 @@
         <v>0</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>4</v>
@@ -4617,19 +4618,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D8" s="11">
         <v>43843</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F8" s="9">
         <v>61</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="38.25">
@@ -4637,22 +4638,22 @@
         <v>2</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D9" s="11">
         <v>43864</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F9" s="9">
         <v>15</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="51">
@@ -4660,22 +4661,22 @@
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D10" s="11">
         <v>43726</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F10" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="N10" t="s">
         <v>204</v>
-      </c>
-      <c r="N10" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="25.5">
@@ -4683,22 +4684,22 @@
         <v>4</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D11" s="11">
         <v>43721</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F11" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="N11" t="s">
         <v>207</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="N11" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="25.5">
@@ -4706,22 +4707,22 @@
         <v>5</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D12" s="11">
         <v>43712</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F12" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="N12" t="s">
         <v>210</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="N12" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="25.5">
@@ -4729,22 +4730,22 @@
         <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D13" s="11">
         <v>43704</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="N13" t="s">
         <v>213</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="N13" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="14" spans="2:16">
@@ -4752,22 +4753,22 @@
         <v>7</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D14" s="11">
         <v>43487</v>
       </c>
       <c r="E14" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="N14" t="s">
         <v>217</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="N14" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="15" spans="2:16">
@@ -4780,12 +4781,12 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="N15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="2:16">
       <c r="N16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="2:7">
@@ -4800,13 +4801,13 @@
         <v>0</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>4</v>
@@ -4820,19 +4821,19 @@
         <v>1</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D20" s="11">
         <v>43342</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F20" s="9">
         <v>58</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="25.5">
@@ -4840,19 +4841,19 @@
         <v>2</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D21" s="11">
         <v>43364</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F21" s="9">
         <v>15</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="25.5">
@@ -4860,19 +4861,19 @@
         <v>3</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D22" s="11">
         <v>43355</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F22" s="9">
         <v>15</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="63.75">
@@ -4880,19 +4881,19 @@
         <v>4</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D23" s="11">
         <v>43370</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F23" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>203</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="25.5">
@@ -4900,19 +4901,19 @@
         <v>5</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D24" s="11">
         <v>43286</v>
       </c>
       <c r="E24" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>227</v>
-      </c>
       <c r="G24" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="2:7">
@@ -4920,19 +4921,19 @@
         <v>6</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D25" s="11">
         <v>43307</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F25" s="9">
         <v>66</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="2:7">
@@ -4940,19 +4941,19 @@
         <v>7</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D26" s="11">
         <v>43321</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="2:7">
@@ -4960,19 +4961,19 @@
         <v>8</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D27" s="11">
         <v>43335</v>
       </c>
       <c r="E27" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="F27" s="9" t="s">
-        <v>234</v>
-      </c>
       <c r="G27" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="2:7">
@@ -4980,19 +4981,19 @@
         <v>9</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D28" s="11">
         <v>43349</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F28" s="9">
         <v>66</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="25.5">
@@ -5000,19 +5001,19 @@
         <v>10</v>
       </c>
       <c r="C29" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="E29" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>239</v>
-      </c>
       <c r="F29" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="2:7">
@@ -5020,19 +5021,19 @@
         <v>11</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D30" s="11">
         <v>43377</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="25.5">
@@ -5040,19 +5041,19 @@
         <v>12</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D31" s="11">
         <v>43358</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F31" s="9">
         <v>69</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="2:7">
@@ -5078,13 +5079,13 @@
         <v>0</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>4</v>
@@ -5098,19 +5099,19 @@
         <v>1</v>
       </c>
       <c r="C38" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="E38" s="9" t="s">
         <v>243</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>244</v>
       </c>
       <c r="F38" s="9">
         <v>55</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="2:7">
@@ -5118,19 +5119,19 @@
         <v>2</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D39" s="11">
         <v>43125</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F39" s="9">
         <v>105</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="2:7">
@@ -5138,19 +5139,19 @@
         <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D40" s="33">
         <v>43157</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F40" s="1">
         <v>45</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="25.5">
@@ -5158,19 +5159,19 @@
         <v>4</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D41" s="33">
         <v>43158</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F41" s="1">
         <v>73</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="2:7">
@@ -5178,19 +5179,19 @@
         <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D42" s="33">
         <v>43120</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="G42" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="30">
@@ -5198,19 +5199,19 @@
         <v>6</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D43" s="33">
         <v>43153</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>254</v>
-      </c>
       <c r="G43" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="30">
@@ -5218,19 +5219,19 @@
         <v>7</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D44" s="33">
         <v>43007</v>
       </c>
       <c r="E44" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="G44" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="25.5">
@@ -5238,19 +5239,19 @@
         <v>8</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D45" s="33">
         <v>43006</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="30">
@@ -5258,19 +5259,19 @@
         <v>9</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D46" s="33">
         <v>43007</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="2:7">
@@ -5278,19 +5279,19 @@
         <v>10</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>262</v>
-      </c>
       <c r="F47" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="2:7">
@@ -5298,19 +5299,19 @@
         <v>11</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D48" s="33">
         <v>42984</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="2:7">
@@ -5323,7 +5324,7 @@
     </row>
     <row r="52" spans="2:7">
       <c r="B52" s="57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C52" s="57"/>
       <c r="D52" s="57"/>
@@ -5333,13 +5334,13 @@
         <v>0</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>4</v>
@@ -5353,19 +5354,19 @@
         <v>1</v>
       </c>
       <c r="C54" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D54" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="E54" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="E54" s="9" t="s">
-        <v>267</v>
-      </c>
       <c r="F54" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="25.5">
@@ -5373,19 +5374,19 @@
         <v>2</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D55" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="E55" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="E55" s="9" t="s">
-        <v>267</v>
-      </c>
       <c r="F55" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="25.5">
@@ -5393,19 +5394,19 @@
         <v>3</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D56" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="E56" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="E56" s="9" t="s">
-        <v>267</v>
-      </c>
       <c r="F56" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="57" spans="2:7">
@@ -5467,7 +5468,7 @@
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="J3" s="59" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K3" s="59"/>
       <c r="L3" s="59"/>
@@ -5477,7 +5478,7 @@
     </row>
     <row r="4" spans="3:15" ht="15.75">
       <c r="D4" s="58" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5519,10 +5520,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>271</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>272</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>2</v>
@@ -5531,7 +5532,7 @@
         <v>32</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="3:15" ht="21.75" customHeight="1">
@@ -5539,19 +5540,19 @@
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="34" t="s">
         <v>275</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="G9" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>277</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="10" spans="3:15">
@@ -5559,19 +5560,19 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E10" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>277</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="11" spans="3:15">
@@ -5579,19 +5580,19 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E11" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G11" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="9" t="s">
         <v>277</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="12" spans="3:15">
@@ -5599,19 +5600,19 @@
         <v>4</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="G12" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>277</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="13" spans="3:15">
@@ -5619,19 +5620,19 @@
         <v>5</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>285</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="14" spans="3:15">
@@ -5639,19 +5640,19 @@
         <v>6</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>285</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="15" spans="3:15">
@@ -5659,19 +5660,19 @@
         <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>288</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>289</v>
       </c>
       <c r="F15" s="36">
         <v>43831</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="3:15">
@@ -5679,19 +5680,19 @@
         <v>8</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>291</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>292</v>
       </c>
       <c r="F16" s="36">
         <v>43831</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="3:16">
@@ -5699,19 +5700,19 @@
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F17" s="36">
         <v>43831</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="3:16" ht="15" customHeight="1">
@@ -5719,19 +5720,19 @@
         <v>10</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="F18" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="19" spans="3:16" ht="18" customHeight="1">
@@ -5739,19 +5740,19 @@
         <v>11</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>302</v>
-      </c>
       <c r="F19" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="20" spans="3:16">
@@ -5759,19 +5760,19 @@
         <v>12</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>303</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>304</v>
       </c>
       <c r="F20" s="28">
         <v>43352</v>
       </c>
       <c r="G20" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="21" spans="3:16">
@@ -5779,19 +5780,19 @@
         <v>13</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="F21" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="H21" s="9" t="s">
         <v>311</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="22" spans="3:16">
@@ -5799,19 +5800,19 @@
         <v>14</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E22" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="H22" s="9" t="s">
         <v>311</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="23" spans="3:16">
@@ -5819,19 +5820,19 @@
         <v>15</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E23" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="H23" s="9" t="s">
         <v>311</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="24" spans="3:16">
@@ -5839,19 +5840,19 @@
         <v>16</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F24" s="28">
         <v>43352</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="3:16">
@@ -5859,17 +5860,17 @@
         <v>17</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>317</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="3:16">
@@ -5877,19 +5878,19 @@
         <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>321</v>
-      </c>
       <c r="H26" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="3:16" ht="15.75">
@@ -5897,17 +5898,17 @@
         <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L27" s="35"/>
       <c r="O27" s="35"/>
@@ -5999,4 +6000,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
C2 Photos of Sports and co-curricular activities at program level added in word file
</commit_message>
<xml_diff>
--- a/C2/C2 NBA All Tables Conso.xlsx
+++ b/C2/C2 NBA All Tables Conso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Personality develop. cell" sheetId="4" r:id="rId1"/>
@@ -1827,7 +1827,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2002,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B59" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2013,7 +2013,7 @@
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" customWidth="1"/>
     <col min="6" max="6" width="45.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
     <col min="9" max="9" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4526,8 +4526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:P57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:P6"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52:G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5438,8 +5438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:P34"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
C2 Students participation in other institute added
</commit_message>
<xml_diff>
--- a/C2/C2 NBA All Tables Conso.xlsx
+++ b/C2/C2 NBA All Tables Conso.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="325">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -1049,6 +1049,15 @@
   </si>
   <si>
     <t>Shree Ramchandra college of engineering,Pune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parandkar G M </t>
+  </si>
+  <si>
+    <t>Error Detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tandale Harshita Pandurang </t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1195,6 +1204,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1378,7 +1399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1477,14 +1498,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1553,6 +1568,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1827,7 +1866,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1850,21 +1889,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="2" t="s">
@@ -1882,11 +1921,11 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
     </row>
     <row r="5" spans="2:12" ht="22.5">
       <c r="B5" s="6">
@@ -2002,7 +2041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L89"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
@@ -2018,26 +2057,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="19.5" customHeight="1">
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="J5" s="42"/>
-      <c r="K5" s="43"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41"/>
     </row>
     <row r="6" spans="2:12" ht="32.25" customHeight="1">
       <c r="B6" s="10" t="s">
@@ -2058,9 +2097,9 @@
       <c r="G6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="46"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="44"/>
     </row>
     <row r="7" spans="2:12" ht="25.5">
       <c r="B7" s="4">
@@ -2081,9 +2120,9 @@
       <c r="G7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="46"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="44"/>
     </row>
     <row r="8" spans="2:12" ht="25.5">
       <c r="B8" s="4">
@@ -2104,9 +2143,9 @@
       <c r="G8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="44"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="44"/>
     </row>
     <row r="9" spans="2:12" ht="25.5">
       <c r="B9" s="4">
@@ -2127,9 +2166,9 @@
       <c r="G9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="47"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="49"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
     </row>
     <row r="10" spans="2:12" ht="25.5">
       <c r="B10" s="4">
@@ -2190,12 +2229,12 @@
       <c r="G12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="40" t="s">
+      <c r="I12" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
     </row>
     <row r="13" spans="2:12" ht="25.5">
       <c r="B13" s="4">
@@ -2216,10 +2255,10 @@
       <c r="G13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
     </row>
     <row r="14" spans="2:12" ht="25.5">
       <c r="B14" s="4">
@@ -2241,7 +2280,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="25.5">
+    <row r="15" spans="2:12">
       <c r="B15" s="4">
         <v>9</v>
       </c>
@@ -2261,7 +2300,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="25.5">
+    <row r="16" spans="2:12">
       <c r="B16" s="4">
         <v>10</v>
       </c>
@@ -2281,7 +2320,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="25.5">
+    <row r="17" spans="2:7">
       <c r="B17" s="4">
         <v>11</v>
       </c>
@@ -2301,7 +2340,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="25.5">
+    <row r="18" spans="2:7">
       <c r="B18" s="4">
         <v>12</v>
       </c>
@@ -2341,7 +2380,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="25.5">
+    <row r="20" spans="2:7">
       <c r="B20" s="4">
         <v>14</v>
       </c>
@@ -2378,11 +2417,11 @@
       <c r="G22" s="19"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -2928,10 +2967,10 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B54" s="39" t="s">
+      <c r="B54" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="39"/>
+      <c r="C54" s="37"/>
     </row>
     <row r="55" spans="2:7" ht="25.5">
       <c r="B55" s="22" t="s">
@@ -3154,11 +3193,11 @@
       </c>
     </row>
     <row r="69" spans="2:7" ht="15.75">
-      <c r="B69" s="39" t="s">
+      <c r="B69" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="C69" s="39"/>
-      <c r="D69" s="39"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37"/>
     </row>
     <row r="70" spans="2:7" ht="25.5">
       <c r="B70" s="22" t="s">
@@ -3594,13 +3633,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" customHeight="1">
       <c r="B2" s="12"/>
@@ -3608,43 +3647,43 @@
       <c r="D2" s="25"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="43"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="41"/>
     </row>
     <row r="3" spans="1:15" ht="15.75">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="49"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="47"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
     </row>
     <row r="6" spans="1:15" ht="51.75" customHeight="1">
       <c r="A6" s="10" t="s">
@@ -3975,14 +4014,14 @@
       <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
     </row>
     <row r="24" spans="1:6" ht="51">
       <c r="A24" s="10" t="s">
@@ -4241,14 +4280,14 @@
       <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="52" t="s">
+      <c r="A38" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="54"/>
+      <c r="B38" s="51"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="52"/>
     </row>
     <row r="39" spans="1:6" ht="38.25">
       <c r="A39" s="10" t="s">
@@ -4380,13 +4419,13 @@
     </row>
     <row r="46" spans="1:6" ht="24.95" customHeight="1">
       <c r="A46" s="2"/>
-      <c r="B46" s="52" t="s">
+      <c r="B46" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
     </row>
     <row r="47" spans="1:6" ht="38.25">
       <c r="A47" s="10" t="s">
@@ -4526,7 +4565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:P57"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B52" sqref="B52:G56"/>
     </sheetView>
   </sheetViews>
@@ -4542,13 +4581,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="19.5">
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
     </row>
     <row r="3" spans="2:16" ht="19.5">
       <c r="C3" s="13"/>
@@ -4558,40 +4597,40 @@
       <c r="G3" s="13"/>
     </row>
     <row r="4" spans="2:16" ht="15.75">
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="56" t="s">
         <v>269</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
     </row>
     <row r="5" spans="2:16">
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="43"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="41"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="49"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="47"/>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" s="10" t="s">
@@ -4790,11 +4829,11 @@
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="10" t="s">
@@ -5068,11 +5107,11 @@
       <c r="C33" s="32"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
     </row>
     <row r="37" spans="2:7">
       <c r="B37" s="10" t="s">
@@ -5323,11 +5362,11 @@
       <c r="G49" s="1"/>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="57" t="s">
+      <c r="B52" s="55" t="s">
         <v>184</v>
       </c>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57"/>
+      <c r="C52" s="55"/>
+      <c r="D52" s="55"/>
     </row>
     <row r="53" spans="2:7">
       <c r="B53" s="10" t="s">
@@ -5436,10 +5475,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:P34"/>
+  <dimension ref="C2:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5453,13 +5492,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:15" ht="19.5">
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
     </row>
     <row r="3" spans="3:15" ht="19.5">
       <c r="D3" s="13"/>
@@ -5467,85 +5506,97 @@
       <c r="F3" s="25"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="57" t="s">
         <v>314</v>
       </c>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
     </row>
     <row r="4" spans="3:15" ht="15.75">
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="56" t="s">
         <v>306</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
     </row>
     <row r="5" spans="3:15">
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
     </row>
     <row r="6" spans="3:15">
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-    </row>
-    <row r="7" spans="3:15">
-      <c r="C7" s="57" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-    </row>
-    <row r="8" spans="3:15" ht="24" customHeight="1">
-      <c r="C8" s="10" t="s">
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
+    </row>
+    <row r="7" spans="3:15" ht="24" customHeight="1">
+      <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="3:15" ht="21.75" customHeight="1">
-      <c r="C9" s="9">
+    <row r="8" spans="3:15" ht="21.75" customHeight="1">
+      <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>273</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F8" s="64" t="s">
+        <v>275</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15">
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>278</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="65" t="s">
         <v>275</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -5556,16 +5607,16 @@
       </c>
     </row>
     <row r="10" spans="3:15">
-      <c r="C10" s="1">
-        <v>2</v>
+      <c r="C10" s="9">
+        <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="65" t="s">
         <v>275</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -5576,16 +5627,16 @@
       </c>
     </row>
     <row r="11" spans="3:15">
-      <c r="C11" s="9">
-        <v>3</v>
+      <c r="C11" s="1">
+        <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="65" t="s">
         <v>275</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -5596,36 +5647,36 @@
       </c>
     </row>
     <row r="12" spans="3:15">
-      <c r="C12" s="1">
-        <v>4</v>
+      <c r="C12" s="9">
+        <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>277</v>
+        <v>281</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F12" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="3:15">
-      <c r="C13" s="9">
-        <v>5</v>
+      <c r="C13" s="1">
+        <v>6</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="58" t="s">
         <v>283</v>
       </c>
       <c r="G13" s="4" t="s">
@@ -5636,96 +5687,96 @@
       </c>
     </row>
     <row r="14" spans="3:15">
-      <c r="C14" s="1">
-        <v>6</v>
+      <c r="C14" s="9">
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>284</v>
+        <v>288</v>
+      </c>
+      <c r="F14" s="59">
+        <v>43831</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="3:15">
-      <c r="C15" s="9">
-        <v>7</v>
+      <c r="C15" s="1">
+        <v>8</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="F15" s="36">
+        <v>291</v>
+      </c>
+      <c r="F15" s="59">
         <v>43831</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>276</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="3:15">
-      <c r="C16" s="1">
-        <v>8</v>
+      <c r="C16" s="9">
+        <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="F16" s="36">
+        <v>293</v>
+      </c>
+      <c r="F16" s="59">
         <v>43831</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>276</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="17" spans="3:16">
-      <c r="C17" s="9">
-        <v>9</v>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" ht="15" customHeight="1">
+      <c r="C17" s="1">
+        <v>10</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="F17" s="36">
-        <v>43831</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>276</v>
+        <v>295</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>297</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>298</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="18" spans="3:16" ht="15" customHeight="1">
-      <c r="C18" s="1">
-        <v>10</v>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" ht="18" customHeight="1">
+      <c r="C18" s="9">
+        <v>11</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="F18" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F18" s="60" t="s">
         <v>297</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -5735,57 +5786,57 @@
         <v>299</v>
       </c>
     </row>
-    <row r="19" spans="3:16" ht="18" customHeight="1">
-      <c r="C19" s="9">
-        <v>11</v>
+    <row r="19" spans="3:16">
+      <c r="C19" s="1">
+        <v>12</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>297</v>
+        <v>302</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F19" s="61">
+        <v>43352</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="3:16">
-      <c r="C20" s="1">
-        <v>12</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="F20" s="28">
-        <v>43352</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>305</v>
+      <c r="C20" s="9">
+        <v>13</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F20" s="62" t="s">
+        <v>310</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="3:16">
-      <c r="C21" s="9">
-        <v>13</v>
+      <c r="C21" s="1">
+        <v>14</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="62" t="s">
         <v>310</v>
       </c>
       <c r="G21" s="9" t="s">
@@ -5796,16 +5847,16 @@
       </c>
     </row>
     <row r="22" spans="3:16">
-      <c r="C22" s="1">
-        <v>14</v>
+      <c r="C22" s="9">
+        <v>15</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="62" t="s">
         <v>310</v>
       </c>
       <c r="G22" s="9" t="s">
@@ -5816,133 +5867,147 @@
       </c>
     </row>
     <row r="23" spans="3:16">
-      <c r="C23" s="9">
-        <v>15</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>310</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>311</v>
+      <c r="C23" s="1">
+        <v>16</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F23" s="61">
+        <v>43352</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="24" spans="3:16">
-      <c r="C24" s="1">
-        <v>16</v>
+      <c r="C24" s="9">
+        <v>17</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="F24" s="28">
-        <v>43352</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>304</v>
+      <c r="E24" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F24" s="63">
+        <v>43120</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="25" spans="3:16">
-      <c r="C25" s="9">
-        <v>17</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>315</v>
+      <c r="C25" s="1">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>318</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>319</v>
+      </c>
+      <c r="F25" s="60" t="s">
+        <v>297</v>
+      </c>
       <c r="G25" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="26" spans="3:16">
-      <c r="C26" s="1">
-        <v>18</v>
+        <v>320</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="26" spans="3:16" ht="15.75">
+      <c r="C26" s="9">
+        <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>318</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>297</v>
+        <v>316</v>
+      </c>
+      <c r="F26" s="63">
+        <v>43120</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>311</v>
       </c>
+      <c r="L26" s="34"/>
+      <c r="O26" s="34"/>
+      <c r="P26" s="34"/>
     </row>
     <row r="27" spans="3:16" ht="15.75">
-      <c r="C27" s="9">
-        <v>19</v>
+      <c r="C27" s="1">
+        <v>20</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>323</v>
+      </c>
+      <c r="F27" s="60" t="s">
+        <v>297</v>
+      </c>
       <c r="G27" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="L27" s="35"/>
-      <c r="O27" s="35"/>
-      <c r="P27" s="35"/>
+      <c r="L27" s="34"/>
+      <c r="O27" s="34"/>
+      <c r="P27" s="34"/>
     </row>
     <row r="28" spans="3:16" ht="15.75">
-      <c r="C28" s="1">
-        <v>20</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="L28" s="35"/>
-      <c r="O28" s="35"/>
-      <c r="P28" s="35"/>
-    </row>
-    <row r="29" spans="3:16" ht="15.75">
-      <c r="C29" s="9">
+      <c r="C28" s="9">
         <v>21</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F28" s="61">
+        <v>43352</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="L28" s="34"/>
+      <c r="O28" s="34"/>
+      <c r="P28" s="34"/>
+    </row>
+    <row r="29" spans="3:16">
+      <c r="C29" s="1">
+        <v>22</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="L29" s="35"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="35"/>
     </row>
     <row r="30" spans="3:16">
-      <c r="C30" s="1">
-        <v>22</v>
+      <c r="C30" s="9">
+        <v>23</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -5951,8 +6016,8 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="3:16">
-      <c r="C31" s="9">
-        <v>23</v>
+      <c r="C31" s="1">
+        <v>24</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -5961,8 +6026,8 @@
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="3:16">
-      <c r="C32" s="1">
-        <v>24</v>
+      <c r="C32" s="9">
+        <v>25</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -5971,8 +6036,8 @@
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="3:8">
-      <c r="C33" s="9">
-        <v>25</v>
+      <c r="C33" s="1">
+        <v>26</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -5980,20 +6045,449 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="3:8">
-      <c r="C34" s="1">
-        <v>26</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+    <row r="36" spans="3:8">
+      <c r="C36" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8">
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F37" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8">
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F38" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8">
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F39" s="59">
+        <v>43831</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8">
+      <c r="C40" s="1">
+        <v>4</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F40" s="59">
+        <v>43831</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8">
+      <c r="C41" s="1">
+        <v>5</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="F41" s="59">
+        <v>43831</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8">
+      <c r="C42" s="1">
+        <v>6</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="F42" s="60" t="s">
+        <v>297</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8">
+      <c r="C43" s="1">
+        <v>7</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="F43" s="60" t="s">
+        <v>297</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8">
+      <c r="C44" s="1">
+        <v>8</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F44" s="61">
+        <v>43352</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8">
+      <c r="C45" s="1">
+        <v>9</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F45" s="62" t="s">
+        <v>310</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8">
+      <c r="C46" s="1">
+        <v>10</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F46" s="62" t="s">
+        <v>310</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8">
+      <c r="C47" s="1">
+        <v>11</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F47" s="62" t="s">
+        <v>310</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8">
+      <c r="C48" s="1">
+        <v>12</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F48" s="61">
+        <v>43352</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8">
+      <c r="C49" s="1">
+        <v>13</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F49" s="63">
+        <v>43120</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8">
+      <c r="C50" s="1">
+        <v>14</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F50" s="60" t="s">
+        <v>297</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8">
+      <c r="C51" s="1">
+        <v>15</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F51" s="63">
+        <v>43120</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8">
+      <c r="C52" s="1">
+        <v>16</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F52" s="60" t="s">
+        <v>297</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8">
+      <c r="C53" s="1">
+        <v>17</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F53" s="61">
+        <v>43352</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8">
+      <c r="C54" s="1">
+        <v>18</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F54" s="64" t="s">
+        <v>275</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8">
+      <c r="C55" s="1">
+        <v>19</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F55" s="65" t="s">
+        <v>275</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8">
+      <c r="C56" s="1">
+        <v>20</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F56" s="65" t="s">
+        <v>275</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8">
+      <c r="C57" s="1">
+        <v>21</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F57" s="65" t="s">
+        <v>275</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>277</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="J3:O6"/>
-    <mergeCell ref="C7:F7"/>
     <mergeCell ref="D2:H2"/>
     <mergeCell ref="D4:H4"/>
   </mergeCells>

</xml_diff>

<commit_message>
C2 Orientation activity added in Excel sheet and word file
</commit_message>
<xml_diff>
--- a/C2/C2 NBA All Tables Conso.xlsx
+++ b/C2/C2 NBA All Tables Conso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Personality develop. cell" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="328">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -1059,6 +1059,15 @@
   <si>
     <t xml:space="preserve">Tandale Harshita Pandurang </t>
   </si>
+  <si>
+    <t>MSBTE Live Webinar on Emerging trends in Computer Engg</t>
+  </si>
+  <si>
+    <t>MSBTE Expert Person</t>
+  </si>
+  <si>
+    <t>Live-State Level Orientation activity</t>
+  </si>
 </sst>
 </file>
 
@@ -1067,7 +1076,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1181,6 +1190,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1220,7 +1235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1395,11 +1410,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1501,6 +1529,30 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1570,28 +1622,19 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1889,21 +1932,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="2" t="s">
@@ -1921,11 +1964,11 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
     </row>
     <row r="5" spans="2:12" ht="22.5">
       <c r="B5" s="6">
@@ -2057,26 +2100,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="19.5" customHeight="1">
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
-      <c r="I5" s="39" t="s">
+      <c r="I5" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="41"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="49"/>
     </row>
     <row r="6" spans="2:12" ht="32.25" customHeight="1">
       <c r="B6" s="10" t="s">
@@ -2097,9 +2140,9 @@
       <c r="G6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="52"/>
     </row>
     <row r="7" spans="2:12" ht="25.5">
       <c r="B7" s="4">
@@ -2120,9 +2163,9 @@
       <c r="G7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="44"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="52"/>
     </row>
     <row r="8" spans="2:12" ht="25.5">
       <c r="B8" s="4">
@@ -2143,9 +2186,9 @@
       <c r="G8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="44"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="52"/>
     </row>
     <row r="9" spans="2:12" ht="25.5">
       <c r="B9" s="4">
@@ -2166,9 +2209,9 @@
       <c r="G9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="45"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="47"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="55"/>
     </row>
     <row r="10" spans="2:12" ht="25.5">
       <c r="B10" s="4">
@@ -2229,12 +2272,12 @@
       <c r="G12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" spans="2:12" ht="25.5">
       <c r="B13" s="4">
@@ -2255,10 +2298,10 @@
       <c r="G13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
     </row>
     <row r="14" spans="2:12" ht="25.5">
       <c r="B14" s="4">
@@ -2417,11 +2460,11 @@
       <c r="G22" s="19"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -2967,10 +3010,10 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B54" s="37" t="s">
+      <c r="B54" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="37"/>
+      <c r="C54" s="45"/>
     </row>
     <row r="55" spans="2:7" ht="25.5">
       <c r="B55" s="22" t="s">
@@ -3193,11 +3236,11 @@
       </c>
     </row>
     <row r="69" spans="2:7" ht="15.75">
-      <c r="B69" s="37" t="s">
+      <c r="B69" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="C69" s="37"/>
-      <c r="D69" s="37"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="45"/>
     </row>
     <row r="70" spans="2:7" ht="25.5">
       <c r="B70" s="22" t="s">
@@ -3633,13 +3676,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" customHeight="1">
       <c r="B2" s="12"/>
@@ -3647,43 +3690,43 @@
       <c r="D2" s="25"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="41"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="49"/>
     </row>
     <row r="3" spans="1:15" ht="15.75">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="47"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="55"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" spans="1:15" ht="51.75" customHeight="1">
       <c r="A6" s="10" t="s">
@@ -4014,14 +4057,14 @@
       <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
     </row>
     <row r="24" spans="1:6" ht="51">
       <c r="A24" s="10" t="s">
@@ -4280,14 +4323,14 @@
       <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="51"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="52"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="60"/>
     </row>
     <row r="39" spans="1:6" ht="38.25">
       <c r="A39" s="10" t="s">
@@ -4419,13 +4462,13 @@
     </row>
     <row r="46" spans="1:6" ht="24.95" customHeight="1">
       <c r="A46" s="2"/>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
     </row>
     <row r="47" spans="1:6" ht="38.25">
       <c r="A47" s="10" t="s">
@@ -4563,16 +4606,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:P57"/>
+  <dimension ref="B2:P58"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52:G56"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" customWidth="1"/>
+    <col min="3" max="3" width="57.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="46.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
@@ -4581,13 +4624,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="19.5">
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="2:16" ht="19.5">
       <c r="C3" s="13"/>
@@ -4597,42 +4640,42 @@
       <c r="G3" s="13"/>
     </row>
     <row r="4" spans="2:16" ht="15.75">
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="64" t="s">
         <v>269</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
     </row>
     <row r="5" spans="2:16">
-      <c r="I5" s="39" t="s">
+      <c r="I5" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="41"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="49"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="47"/>
-    </row>
-    <row r="7" spans="2:16">
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="55"/>
+    </row>
+    <row r="7" spans="2:16" ht="25.5">
       <c r="B7" s="10" t="s">
         <v>0</v>
       </c>
@@ -4652,93 +4695,90 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="25.5">
+    <row r="8" spans="2:16" ht="30">
       <c r="B8" s="9">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="68" t="s">
+        <v>325</v>
+      </c>
+      <c r="D8" s="69">
+        <v>43834</v>
+      </c>
+      <c r="E8" s="70" t="s">
+        <v>326</v>
+      </c>
+      <c r="F8" s="70">
+        <v>55</v>
+      </c>
+      <c r="G8" s="70" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="25.5">
+      <c r="B9" s="66">
+        <v>2</v>
+      </c>
+      <c r="C9" s="66" t="s">
         <v>195</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D9" s="67">
         <v>43843</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E9" s="66" t="s">
         <v>196</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F9" s="66">
         <v>61</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G9" s="66" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="38.25">
-      <c r="B9" s="9">
-        <v>2</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="D9" s="11">
-        <v>43864</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="F9" s="9">
-        <v>15</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="N9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" ht="51">
+    <row r="10" spans="2:16" ht="38.25">
       <c r="B10" s="9">
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D10" s="11">
-        <v>43726</v>
+        <v>43864</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
+      </c>
+      <c r="F10" s="9">
+        <v>15</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="N10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" ht="25.5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="51">
       <c r="B11" s="9">
         <v>4</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D11" s="11">
-        <v>43721</v>
+        <v>43726</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>196</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>203</v>
       </c>
       <c r="N11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="25.5">
@@ -4746,22 +4786,22 @@
         <v>5</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D12" s="11">
-        <v>43712</v>
+        <v>43721</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>196</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>203</v>
       </c>
       <c r="N12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="25.5">
@@ -4769,141 +4809,144 @@
         <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D13" s="11">
-        <v>43704</v>
+        <v>43712</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>196</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>203</v>
       </c>
       <c r="N13" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="25.5">
       <c r="B14" s="9">
         <v>7</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D14" s="11">
-        <v>43487</v>
+        <v>43704</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>203</v>
       </c>
       <c r="N14" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="2:16">
       <c r="B15" s="9">
         <v>8</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="C15" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D15" s="11">
+        <v>43487</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="N15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
+      <c r="B16" s="9">
+        <v>9</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="N16" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
-      <c r="N16" t="s">
+    <row r="17" spans="2:14">
+      <c r="N17" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="55" t="s">
+    <row r="19" spans="2:14">
+      <c r="B19" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="10" t="s">
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F20" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="9">
+    <row r="21" spans="2:14">
+      <c r="B21" s="9">
         <v>1</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D21" s="11">
         <v>43342</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E21" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F21" s="9">
         <v>58</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="25.5">
-      <c r="B21" s="9">
-        <v>2</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="D21" s="11">
-        <v>43364</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="F21" s="9">
-        <v>15</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="25.5">
+    <row r="22" spans="2:14" ht="25.5">
       <c r="B22" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="D22" s="11">
-        <v>43355</v>
+        <v>43364</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>196</v>
@@ -4915,158 +4958,158 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="63.75">
+    <row r="23" spans="2:14" ht="25.5">
       <c r="B23" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D23" s="11">
-        <v>43370</v>
+        <v>43355</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>202</v>
+      <c r="F23" s="9">
+        <v>15</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="25.5">
+    <row r="24" spans="2:14" ht="63.75">
       <c r="B24" s="9">
+        <v>4</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D24" s="11">
+        <v>43370</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="25.5">
+      <c r="B25" s="9">
         <v>5</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D25" s="11">
         <v>43286</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E25" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F25" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="9">
-        <v>6</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="D25" s="11">
-        <v>43307</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="F25" s="9">
-        <v>66</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:14">
       <c r="B26" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D26" s="11">
-        <v>43321</v>
+        <v>43307</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>226</v>
+        <v>228</v>
+      </c>
+      <c r="F26" s="9">
+        <v>66</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:14">
       <c r="B27" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D27" s="11">
-        <v>43335</v>
+        <v>43321</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="2:7">
+    <row r="28" spans="2:14">
       <c r="B28" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D28" s="11">
-        <v>43349</v>
+        <v>43335</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="F28" s="9">
-        <v>66</v>
+        <v>232</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="25.5">
+    <row r="29" spans="2:14">
       <c r="B29" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>237</v>
+        <v>234</v>
+      </c>
+      <c r="D29" s="11">
+        <v>43349</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>226</v>
+        <v>235</v>
+      </c>
+      <c r="F29" s="9">
+        <v>66</v>
       </c>
       <c r="G29" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:14" ht="25.5">
       <c r="B30" s="9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="D30" s="11">
-        <v>43377</v>
+        <v>236</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>237</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>226</v>
@@ -5075,233 +5118,233 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="25.5">
+    <row r="31" spans="2:14">
       <c r="B31" s="9">
+        <v>11</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D31" s="11">
+        <v>43377</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" ht="25.5">
+      <c r="B32" s="9">
         <v>12</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C32" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D32" s="11">
         <v>43358</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E32" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F32" s="9">
         <v>69</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G32" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="2:7">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-    </row>
     <row r="33" spans="2:7">
-      <c r="C33" s="32"/>
-    </row>
-    <row r="36" spans="2:7">
-      <c r="B36" s="55" t="s">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="C34" s="32"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-    </row>
-    <row r="37" spans="2:7">
-      <c r="B37" s="10" t="s">
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F38" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G38" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="25.5">
-      <c r="B38" s="9">
+    <row r="39" spans="2:7" ht="25.5">
+      <c r="B39" s="9">
         <v>1</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E39" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F39" s="9">
         <v>55</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G39" s="9" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="39" spans="2:7">
-      <c r="B39" s="9">
+    <row r="40" spans="2:7">
+      <c r="B40" s="9">
         <v>2</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C40" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D40" s="11">
         <v>43125</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="F39" s="9">
-        <v>105</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7">
-      <c r="B40" s="1">
-        <v>3</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D40" s="33">
-        <v>43157</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="F40" s="1">
-        <v>45</v>
+      <c r="F40" s="9">
+        <v>105</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="25.5">
-      <c r="B41" s="9">
-        <v>4</v>
+    <row r="41" spans="2:7">
+      <c r="B41" s="1">
+        <v>3</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D41" s="33">
-        <v>43158</v>
+        <v>43157</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>196</v>
+        <v>245</v>
       </c>
       <c r="F41" s="1">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="2:7">
+    <row r="42" spans="2:7" ht="25.5">
       <c r="B42" s="9">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D42" s="33">
+        <v>43158</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="F42" s="1">
+        <v>73</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" s="9">
         <v>5</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D42" s="33">
+      <c r="D43" s="33">
         <v>43120</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="30">
-      <c r="B43" s="1">
-        <v>6</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="D43" s="33">
-        <v>43153</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="30">
-      <c r="B44" s="9">
+      <c r="B44" s="1">
+        <v>6</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D44" s="33">
+        <v>43153</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="30">
+      <c r="B45" s="9">
         <v>7</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="D44" s="33">
+      <c r="D45" s="33">
         <v>43007</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" ht="25.5">
-      <c r="B45" s="9">
-        <v>8</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D45" s="33">
-        <v>43006</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="2:7" ht="30">
-      <c r="B46" s="1">
-        <v>9</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>258</v>
+    <row r="46" spans="2:7" ht="25.5">
+      <c r="B46" s="9">
+        <v>8</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>257</v>
       </c>
       <c r="D46" s="33">
-        <v>43007</v>
+        <v>43006</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>196</v>
@@ -5313,21 +5356,21 @@
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="2:7">
+    <row r="47" spans="2:7" ht="30">
       <c r="B47" s="1">
-        <v>10</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>261</v>
+        <v>9</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="33">
+        <v>43007</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>196</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="G47" s="9" t="s">
         <v>203</v>
@@ -5335,16 +5378,16 @@
     </row>
     <row r="48" spans="2:7">
       <c r="B48" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D48" s="33">
-        <v>42984</v>
+        <v>259</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>253</v>
@@ -5354,66 +5397,66 @@
       </c>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="52" spans="2:7">
-      <c r="B52" s="55" t="s">
+      <c r="B49" s="1">
+        <v>11</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D49" s="33">
+        <v>42984</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="53" spans="2:7">
+      <c r="B53" s="63" t="s">
         <v>184</v>
       </c>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-    </row>
-    <row r="53" spans="2:7">
-      <c r="B53" s="10" t="s">
+      <c r="C53" s="63"/>
+      <c r="D53" s="63"/>
+    </row>
+    <row r="54" spans="2:7">
+      <c r="B54" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C54" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D54" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E54" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F54" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G53" s="10" t="s">
+      <c r="G54" s="10" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" ht="25.5">
-      <c r="B54" s="9">
-        <v>1</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="25.5">
       <c r="B55" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>265</v>
@@ -5429,11 +5472,11 @@
       </c>
     </row>
     <row r="56" spans="2:7" ht="25.5">
-      <c r="B56" s="1">
-        <v>3</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>268</v>
+      <c r="B56" s="9">
+        <v>2</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>267</v>
       </c>
       <c r="D56" s="11" t="s">
         <v>265</v>
@@ -5441,32 +5484,52 @@
       <c r="E56" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F56" s="9" t="s">
         <v>216</v>
       </c>
       <c r="G56" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="57" spans="2:7">
-      <c r="B57" s="9">
+    <row r="57" spans="2:7" ht="25.5">
+      <c r="B57" s="1">
+        <v>3</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7">
+      <c r="B58" s="9">
         <v>4</v>
       </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="9"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B53:D53"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="I5:P6"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5477,7 +5540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C36" sqref="C36:H57"/>
     </sheetView>
   </sheetViews>
@@ -5492,13 +5555,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:15" ht="19.5">
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
     </row>
     <row r="3" spans="3:15" ht="19.5">
       <c r="D3" s="13"/>
@@ -5506,45 +5569,45 @@
       <c r="F3" s="25"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="65" t="s">
         <v>314</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
     </row>
     <row r="4" spans="3:15" ht="15.75">
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="64" t="s">
         <v>306</v>
       </c>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
     </row>
     <row r="5" spans="3:15">
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
     </row>
     <row r="6" spans="3:15">
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
-      <c r="O6" s="57"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
     </row>
     <row r="7" spans="3:15" ht="24" customHeight="1">
       <c r="C7" s="10" t="s">
@@ -5576,7 +5639,7 @@
       <c r="E8" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F8" s="64" t="s">
+      <c r="F8" s="41" t="s">
         <v>275</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -5596,7 +5659,7 @@
       <c r="E9" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F9" s="65" t="s">
+      <c r="F9" s="42" t="s">
         <v>275</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -5616,7 +5679,7 @@
       <c r="E10" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F10" s="65" t="s">
+      <c r="F10" s="42" t="s">
         <v>275</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -5636,7 +5699,7 @@
       <c r="E11" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="42" t="s">
         <v>275</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -5656,7 +5719,7 @@
       <c r="E12" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="F12" s="58" t="s">
+      <c r="F12" s="35" t="s">
         <v>283</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -5676,7 +5739,7 @@
       <c r="E13" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="F13" s="58" t="s">
+      <c r="F13" s="35" t="s">
         <v>283</v>
       </c>
       <c r="G13" s="4" t="s">
@@ -5696,7 +5759,7 @@
       <c r="E14" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="F14" s="59">
+      <c r="F14" s="36">
         <v>43831</v>
       </c>
       <c r="G14" s="9" t="s">
@@ -5716,7 +5779,7 @@
       <c r="E15" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="F15" s="59">
+      <c r="F15" s="36">
         <v>43831</v>
       </c>
       <c r="G15" s="9" t="s">
@@ -5736,7 +5799,7 @@
       <c r="E16" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="F16" s="59">
+      <c r="F16" s="36">
         <v>43831</v>
       </c>
       <c r="G16" s="9" t="s">
@@ -5756,7 +5819,7 @@
       <c r="E17" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="F17" s="60" t="s">
+      <c r="F17" s="37" t="s">
         <v>297</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -5776,7 +5839,7 @@
       <c r="E18" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="37" t="s">
         <v>297</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -5796,7 +5859,7 @@
       <c r="E19" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F19" s="61">
+      <c r="F19" s="38">
         <v>43352</v>
       </c>
       <c r="G19" s="4" t="s">
@@ -5816,7 +5879,7 @@
       <c r="E20" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="F20" s="62" t="s">
+      <c r="F20" s="39" t="s">
         <v>310</v>
       </c>
       <c r="G20" s="9" t="s">
@@ -5836,7 +5899,7 @@
       <c r="E21" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="F21" s="62" t="s">
+      <c r="F21" s="39" t="s">
         <v>310</v>
       </c>
       <c r="G21" s="9" t="s">
@@ -5856,7 +5919,7 @@
       <c r="E22" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="F22" s="62" t="s">
+      <c r="F22" s="39" t="s">
         <v>310</v>
       </c>
       <c r="G22" s="9" t="s">
@@ -5876,7 +5939,7 @@
       <c r="E23" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F23" s="61">
+      <c r="F23" s="38">
         <v>43352</v>
       </c>
       <c r="G23" s="4" t="s">
@@ -5896,7 +5959,7 @@
       <c r="E24" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="F24" s="63">
+      <c r="F24" s="40">
         <v>43120</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -5916,7 +5979,7 @@
       <c r="E25" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="F25" s="60" t="s">
+      <c r="F25" s="37" t="s">
         <v>297</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -5936,7 +5999,7 @@
       <c r="E26" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="F26" s="63">
+      <c r="F26" s="40">
         <v>43120</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -5959,7 +6022,7 @@
       <c r="E27" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="F27" s="60" t="s">
+      <c r="F27" s="37" t="s">
         <v>297</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -5982,7 +6045,7 @@
       <c r="E28" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F28" s="61">
+      <c r="F28" s="38">
         <v>43352</v>
       </c>
       <c r="G28" s="4" t="s">
@@ -6075,7 +6138,7 @@
       <c r="E37" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="F37" s="58" t="s">
+      <c r="F37" s="35" t="s">
         <v>283</v>
       </c>
       <c r="G37" s="4" t="s">
@@ -6095,7 +6158,7 @@
       <c r="E38" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="F38" s="58" t="s">
+      <c r="F38" s="35" t="s">
         <v>283</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -6115,7 +6178,7 @@
       <c r="E39" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="F39" s="59">
+      <c r="F39" s="36">
         <v>43831</v>
       </c>
       <c r="G39" s="9" t="s">
@@ -6135,7 +6198,7 @@
       <c r="E40" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="F40" s="59">
+      <c r="F40" s="36">
         <v>43831</v>
       </c>
       <c r="G40" s="9" t="s">
@@ -6155,7 +6218,7 @@
       <c r="E41" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="F41" s="59">
+      <c r="F41" s="36">
         <v>43831</v>
       </c>
       <c r="G41" s="9" t="s">
@@ -6175,7 +6238,7 @@
       <c r="E42" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="F42" s="60" t="s">
+      <c r="F42" s="37" t="s">
         <v>297</v>
       </c>
       <c r="G42" s="4" t="s">
@@ -6195,7 +6258,7 @@
       <c r="E43" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="F43" s="60" t="s">
+      <c r="F43" s="37" t="s">
         <v>297</v>
       </c>
       <c r="G43" s="4" t="s">
@@ -6215,7 +6278,7 @@
       <c r="E44" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F44" s="61">
+      <c r="F44" s="38">
         <v>43352</v>
       </c>
       <c r="G44" s="4" t="s">
@@ -6235,7 +6298,7 @@
       <c r="E45" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="F45" s="62" t="s">
+      <c r="F45" s="39" t="s">
         <v>310</v>
       </c>
       <c r="G45" s="9" t="s">
@@ -6255,7 +6318,7 @@
       <c r="E46" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="F46" s="62" t="s">
+      <c r="F46" s="39" t="s">
         <v>310</v>
       </c>
       <c r="G46" s="9" t="s">
@@ -6275,7 +6338,7 @@
       <c r="E47" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="F47" s="62" t="s">
+      <c r="F47" s="39" t="s">
         <v>310</v>
       </c>
       <c r="G47" s="9" t="s">
@@ -6295,7 +6358,7 @@
       <c r="E48" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F48" s="61">
+      <c r="F48" s="38">
         <v>43352</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -6315,7 +6378,7 @@
       <c r="E49" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="F49" s="63">
+      <c r="F49" s="40">
         <v>43120</v>
       </c>
       <c r="G49" s="1" t="s">
@@ -6335,7 +6398,7 @@
       <c r="E50" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="F50" s="60" t="s">
+      <c r="F50" s="37" t="s">
         <v>297</v>
       </c>
       <c r="G50" s="1" t="s">
@@ -6355,7 +6418,7 @@
       <c r="E51" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="F51" s="63">
+      <c r="F51" s="40">
         <v>43120</v>
       </c>
       <c r="G51" s="1" t="s">
@@ -6375,7 +6438,7 @@
       <c r="E52" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="F52" s="60" t="s">
+      <c r="F52" s="37" t="s">
         <v>297</v>
       </c>
       <c r="G52" s="1" t="s">
@@ -6395,7 +6458,7 @@
       <c r="E53" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F53" s="61">
+      <c r="F53" s="38">
         <v>43352</v>
       </c>
       <c r="G53" s="4" t="s">
@@ -6415,7 +6478,7 @@
       <c r="E54" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F54" s="64" t="s">
+      <c r="F54" s="41" t="s">
         <v>275</v>
       </c>
       <c r="G54" s="9" t="s">
@@ -6435,7 +6498,7 @@
       <c r="E55" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F55" s="65" t="s">
+      <c r="F55" s="42" t="s">
         <v>275</v>
       </c>
       <c r="G55" s="9" t="s">
@@ -6455,7 +6518,7 @@
       <c r="E56" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F56" s="65" t="s">
+      <c r="F56" s="42" t="s">
         <v>275</v>
       </c>
       <c r="G56" s="9" t="s">
@@ -6475,7 +6538,7 @@
       <c r="E57" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F57" s="65" t="s">
+      <c r="F57" s="42" t="s">
         <v>275</v>
       </c>
       <c r="G57" s="9" t="s">

</xml_diff>

<commit_message>
C2 2.2.6 List of facilities and description added in excel and word file
</commit_message>
<xml_diff>
--- a/C2/C2 NBA All Tables Conso.xlsx
+++ b/C2/C2 NBA All Tables Conso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Personality develop. cell" sheetId="4" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Hostel Activities" sheetId="8" r:id="rId3"/>
     <sheet name="Activities Organised BY CO dept" sheetId="9" r:id="rId4"/>
     <sheet name="Students Participation in Techn" sheetId="10" r:id="rId5"/>
-    <sheet name="Sports Winner" sheetId="11" r:id="rId6"/>
+    <sheet name="2.2.6" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="355">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -1068,6 +1068,89 @@
   <si>
     <t>Live-State Level Orientation activity</t>
   </si>
+  <si>
+    <t>Name of Facility</t>
+  </si>
+  <si>
+    <t>Departmental library</t>
+  </si>
+  <si>
+    <t>Video lecture facility</t>
+  </si>
+  <si>
+    <t>Webinar facility</t>
+  </si>
+  <si>
+    <t>NPTEL Videos - Local Storage</t>
+  </si>
+  <si>
+    <t>Seminar-Powerpoint presentation faclity</t>
+  </si>
+  <si>
+    <t>Book Bank facility</t>
+  </si>
+  <si>
+    <t>ICT Enabled Laboratory</t>
+  </si>
+  <si>
+    <t>Delnet libarary network facility</t>
+  </si>
+  <si>
+    <t>The main aim of creating this facility is to faclilitate students to use ICT tools in learning process. This facility will improve knowledge retention among students. This facility helps both students and teachers. Teacher can use resources to enhance the traditional ways of teaching and to keep students more engaged.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reason for creating facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilization </t>
+  </si>
+  <si>
+    <t>Utilized on sharing basis among all three years of classes</t>
+  </si>
+  <si>
+    <t>Internet connecivity in Internet lab, Programming lab,Operating System Lab,Software development lab</t>
+  </si>
+  <si>
+    <t>This facility helps students to get connected to Internet world. Students get more knowledge about recent technological trends, open source softwares and tools,MSBTE educational websites etc. A setup of 70+ Personal Computers is available with Internet facility in each pc for students educational purpose only.</t>
+  </si>
+  <si>
+    <t>Utilized by students of all three years of course</t>
+  </si>
+  <si>
+    <t>The department has books related to the curriculum and
+also some books which will help them to gain extra knowledge. These books are
+issued to the students. These books are used by students for reference purpose.</t>
+  </si>
+  <si>
+    <t>Instutute has active delnet subscription. The Idea behind subscription of DELNET, is to give exposure of worldwide e-contents to students and teachers. Students can get exposure to E-contents, E-books, articles on any topic in any domain. Online Databases, Language learning portal, videos, Ancient Manuscripts and rare books etc are available on DELNET</t>
+  </si>
+  <si>
+    <t>A Setup of Ceiling Mounted Projector, Personal Computer with Internet faclity and Speakers is created so that students can get together and watch video lecttures created by MSBTE / Subject Expert resource person.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSBTE, at state level, organises webinars from time to time for students as well as teachers. </t>
+  </si>
+  <si>
+    <t>Used by teachers and students from institute</t>
+  </si>
+  <si>
+    <t>Utilised at Program level</t>
+  </si>
+  <si>
+    <t>Utilised at Institute  level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two hard-disks contains NPTEL video lectures as local storage.These hard-disks are shared with Electronis department. Video lectures of respective subject are copied on a pc and shown to students </t>
+  </si>
+  <si>
+    <t>Hard-Disk-Drives are utilised on shared basis with Electronics department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This facility helps students to give seminar power point presentation on various topics related to academics as well as their projects. </t>
+  </si>
+  <si>
+    <t>Book bank facility is created at institute level for students. This allows students to use books for a semister and return back books to library after semeser exams are over</t>
+  </si>
 </sst>
 </file>
 
@@ -1076,7 +1159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1193,6 +1276,31 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1427,7 +1535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1553,6 +1661,21 @@
     <xf numFmtId="14" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1622,19 +1745,25 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1909,7 +2038,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1932,21 +2061,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="2" t="s">
@@ -1964,11 +2093,11 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
     </row>
     <row r="5" spans="2:12" ht="22.5">
       <c r="B5" s="6">
@@ -2100,26 +2229,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="19.5" customHeight="1">
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="J5" s="48"/>
-      <c r="K5" s="49"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="54"/>
     </row>
     <row r="6" spans="2:12" ht="32.25" customHeight="1">
       <c r="B6" s="10" t="s">
@@ -2140,9 +2269,9 @@
       <c r="G6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="52"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
     </row>
     <row r="7" spans="2:12" ht="25.5">
       <c r="B7" s="4">
@@ -2163,9 +2292,9 @@
       <c r="G7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="50"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="57"/>
     </row>
     <row r="8" spans="2:12" ht="25.5">
       <c r="B8" s="4">
@@ -2186,9 +2315,9 @@
       <c r="G8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="52"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
     </row>
     <row r="9" spans="2:12" ht="25.5">
       <c r="B9" s="4">
@@ -2209,9 +2338,9 @@
       <c r="G9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="53"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="55"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="60"/>
     </row>
     <row r="10" spans="2:12" ht="25.5">
       <c r="B10" s="4">
@@ -2272,12 +2401,12 @@
       <c r="G12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="46" t="s">
+      <c r="I12" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
     </row>
     <row r="13" spans="2:12" ht="25.5">
       <c r="B13" s="4">
@@ -2298,10 +2427,10 @@
       <c r="G13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
     </row>
     <row r="14" spans="2:12" ht="25.5">
       <c r="B14" s="4">
@@ -2460,11 +2589,11 @@
       <c r="G22" s="19"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -3010,10 +3139,10 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B54" s="45" t="s">
+      <c r="B54" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="45"/>
+      <c r="C54" s="50"/>
     </row>
     <row r="55" spans="2:7" ht="25.5">
       <c r="B55" s="22" t="s">
@@ -3236,11 +3365,11 @@
       </c>
     </row>
     <row r="69" spans="2:7" ht="15.75">
-      <c r="B69" s="45" t="s">
+      <c r="B69" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="C69" s="45"/>
-      <c r="D69" s="45"/>
+      <c r="C69" s="50"/>
+      <c r="D69" s="50"/>
     </row>
     <row r="70" spans="2:7" ht="25.5">
       <c r="B70" s="22" t="s">
@@ -3676,13 +3805,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5">
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" customHeight="1">
       <c r="B2" s="12"/>
@@ -3690,43 +3819,43 @@
       <c r="D2" s="25"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="49"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="54"/>
     </row>
     <row r="3" spans="1:15" ht="15.75">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="55"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="60"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
     </row>
     <row r="6" spans="1:15" ht="51.75" customHeight="1">
       <c r="A6" s="10" t="s">
@@ -4057,14 +4186,14 @@
       <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
     </row>
     <row r="24" spans="1:6" ht="51">
       <c r="A24" s="10" t="s">
@@ -4323,14 +4452,14 @@
       <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="59"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="60"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="65"/>
     </row>
     <row r="39" spans="1:6" ht="38.25">
       <c r="A39" s="10" t="s">
@@ -4462,13 +4591,13 @@
     </row>
     <row r="46" spans="1:6" ht="24.95" customHeight="1">
       <c r="A46" s="2"/>
-      <c r="B46" s="58" t="s">
+      <c r="B46" s="63" t="s">
         <v>184</v>
       </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
+      <c r="C46" s="64"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="64"/>
     </row>
     <row r="47" spans="1:6" ht="38.25">
       <c r="A47" s="10" t="s">
@@ -4608,8 +4737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:G8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4624,13 +4753,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="19.5">
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
     </row>
     <row r="3" spans="2:16" ht="19.5">
       <c r="C3" s="13"/>
@@ -4640,42 +4769,42 @@
       <c r="G3" s="13"/>
     </row>
     <row r="4" spans="2:16" ht="15.75">
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="69" t="s">
         <v>269</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="2:16">
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="49"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="54"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="55"/>
-    </row>
-    <row r="7" spans="2:16" ht="25.5">
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="60"/>
+    </row>
+    <row r="7" spans="2:16">
       <c r="B7" s="10" t="s">
         <v>0</v>
       </c>
@@ -4699,39 +4828,39 @@
       <c r="B8" s="9">
         <v>1</v>
       </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="45" t="s">
         <v>325</v>
       </c>
-      <c r="D8" s="69">
+      <c r="D8" s="46">
         <v>43834</v>
       </c>
-      <c r="E8" s="70" t="s">
+      <c r="E8" s="47" t="s">
         <v>326</v>
       </c>
-      <c r="F8" s="70">
+      <c r="F8" s="47">
         <v>55</v>
       </c>
-      <c r="G8" s="70" t="s">
+      <c r="G8" s="47" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="25.5">
-      <c r="B9" s="66">
+      <c r="B9" s="43">
         <v>2</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="D9" s="67">
+      <c r="D9" s="44">
         <v>43843</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="43" t="s">
         <v>196</v>
       </c>
-      <c r="F9" s="66">
+      <c r="F9" s="43">
         <v>61</v>
       </c>
-      <c r="G9" s="66" t="s">
+      <c r="G9" s="43" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4758,7 +4887,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="51">
+    <row r="11" spans="2:16" ht="38.25">
       <c r="B11" s="9">
         <v>4</v>
       </c>
@@ -4892,11 +5021,11 @@
       </c>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="10" t="s">
@@ -4978,7 +5107,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="2:14" ht="63.75">
+    <row r="24" spans="2:14" ht="51">
       <c r="B24" s="9">
         <v>4</v>
       </c>
@@ -5170,11 +5299,11 @@
       <c r="C34" s="32"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="63" t="s">
+      <c r="B37" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="68"/>
     </row>
     <row r="38" spans="2:7">
       <c r="B38" s="10" t="s">
@@ -5356,7 +5485,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="2:7" ht="30">
+    <row r="47" spans="2:7" ht="25.5">
       <c r="B47" s="1">
         <v>9</v>
       </c>
@@ -5425,11 +5554,11 @@
       <c r="G50" s="1"/>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="63" t="s">
+      <c r="B53" s="68" t="s">
         <v>184</v>
       </c>
-      <c r="C53" s="63"/>
-      <c r="D53" s="63"/>
+      <c r="C53" s="68"/>
+      <c r="D53" s="68"/>
     </row>
     <row r="54" spans="2:7">
       <c r="B54" s="10" t="s">
@@ -5555,13 +5684,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:15" ht="19.5">
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
     </row>
     <row r="3" spans="3:15" ht="19.5">
       <c r="D3" s="13"/>
@@ -5569,45 +5698,45 @@
       <c r="F3" s="25"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="J3" s="65" t="s">
+      <c r="J3" s="70" t="s">
         <v>314</v>
       </c>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
     </row>
     <row r="4" spans="3:15" ht="15.75">
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="69" t="s">
         <v>306</v>
       </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="70"/>
     </row>
     <row r="5" spans="3:15">
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
     </row>
     <row r="6" spans="3:15">
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
     </row>
     <row r="7" spans="3:15" ht="24" customHeight="1">
       <c r="C7" s="10" t="s">
@@ -6561,14 +6690,162 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B4:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="4" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+    <col min="4" max="4" width="76.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:5" ht="39.75" customHeight="1">
+      <c r="B4" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" s="71" t="s">
+        <v>338</v>
+      </c>
+      <c r="E4" s="71" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="62.25" customHeight="1">
+      <c r="B5" s="72">
+        <v>1</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>335</v>
+      </c>
+      <c r="D5" s="74" t="s">
+        <v>337</v>
+      </c>
+      <c r="E5" s="77" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="30">
+      <c r="B6" s="72">
+        <v>2</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>331</v>
+      </c>
+      <c r="D6" s="77" t="s">
+        <v>347</v>
+      </c>
+      <c r="E6" s="77" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="45">
+      <c r="B7" s="75">
+        <v>3</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>330</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>346</v>
+      </c>
+      <c r="E7" s="77" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="60">
+      <c r="B8" s="75">
+        <v>4</v>
+      </c>
+      <c r="C8" s="77" t="s">
+        <v>341</v>
+      </c>
+      <c r="D8" s="77" t="s">
+        <v>342</v>
+      </c>
+      <c r="E8" s="77" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="75">
+      <c r="B9" s="75">
+        <v>5</v>
+      </c>
+      <c r="C9" s="75" t="s">
+        <v>336</v>
+      </c>
+      <c r="D9" s="77" t="s">
+        <v>345</v>
+      </c>
+      <c r="E9" s="77" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="60">
+      <c r="B10" s="75">
+        <v>6</v>
+      </c>
+      <c r="C10" s="75" t="s">
+        <v>329</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>344</v>
+      </c>
+      <c r="E10" s="77" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="49.5" customHeight="1">
+      <c r="B11" s="75">
+        <v>7</v>
+      </c>
+      <c r="C11" s="76" t="s">
+        <v>332</v>
+      </c>
+      <c r="D11" s="77" t="s">
+        <v>351</v>
+      </c>
+      <c r="E11" s="77" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="49.5" customHeight="1">
+      <c r="B12" s="75">
+        <v>8</v>
+      </c>
+      <c r="C12" s="77" t="s">
+        <v>333</v>
+      </c>
+      <c r="D12" s="77" t="s">
+        <v>353</v>
+      </c>
+      <c r="E12" s="77" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="30">
+      <c r="B13" s="75">
+        <v>9</v>
+      </c>
+      <c r="C13" s="76" t="s">
+        <v>334</v>
+      </c>
+      <c r="D13" s="77" t="s">
+        <v>354</v>
+      </c>
+      <c r="E13" s="77" t="s">
+        <v>350</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
C2 2.2.6 A and B Content + Images added in sheet and word file
</commit_message>
<xml_diff>
--- a/C2/C2 NBA All Tables Conso.xlsx
+++ b/C2/C2 NBA All Tables Conso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Personality develop. cell" sheetId="4" r:id="rId1"/>
@@ -12,7 +12,8 @@
     <sheet name="Hostel Activities" sheetId="8" r:id="rId3"/>
     <sheet name="Activities Organised BY CO dept" sheetId="9" r:id="rId4"/>
     <sheet name="Students Participation in Techn" sheetId="10" r:id="rId5"/>
-    <sheet name="2.2.6" sheetId="11" r:id="rId6"/>
+    <sheet name="2.2.6 A" sheetId="11" r:id="rId6"/>
+    <sheet name="2.2.6 B" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="367">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -1150,6 +1151,42 @@
   </si>
   <si>
     <t>Book bank facility is created at institute level for students. This allows students to use books for a semister and return back books to library after semeser exams are over</t>
+  </si>
+  <si>
+    <t>Learning Initiatives Taken</t>
+  </si>
+  <si>
+    <t>Technical Poster Presentation Competition</t>
+  </si>
+  <si>
+    <t>Organizing seminar on Project Topics</t>
+  </si>
+  <si>
+    <t>Quiz competitions on various thrust areas</t>
+  </si>
+  <si>
+    <t>Blind Programming Competitions</t>
+  </si>
+  <si>
+    <t>Encourage students to paprticipate in various state level competitions</t>
+  </si>
+  <si>
+    <t>Used ICT Tools / E-resources / Remarks</t>
+  </si>
+  <si>
+    <t>Students do use Projector and Powerpoint tools for preparing seminar presentations. While Preparing PPT, they can also search more refrences using Ebooks,DELNET library, Expert made PPTs or Journals etc.</t>
+  </si>
+  <si>
+    <t>Technical Poster Presentation competitions allows students to work in team. Find out more information about given topics using ICT technologies. They also learn how to present a topic within given time slot. Generally, topics based on recent technologies like Data Mining, Internet of Things, Cyber Security, Artificial Intelligence etc are given to students so that they do more literature suvey on topics using internet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Projector is used to show questions to students and answer to question are given by students after reading question on screen</t>
+  </si>
+  <si>
+    <t>In this initiative, All monitors are switched off and students are given prgramming problem statement. After a student successfully writes the program,screen is turned on and output of given problem statement is seen on screen. In this, a personal computer set is used by a student indepndantly.</t>
+  </si>
+  <si>
+    <t>Continous encouragement is given to students to participate in various competitions at state level events. All activities like searching for a particular event on college website, applying it etc requires ITC tools.</t>
   </si>
 </sst>
 </file>
@@ -1535,7 +1572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1676,6 +1713,27 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1745,25 +1803,7 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2038,7 +2078,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2061,21 +2101,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="56" t="s">
         <v>187</v>
       </c>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="2" t="s">
@@ -2093,11 +2133,11 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
     </row>
     <row r="5" spans="2:12" ht="22.5">
       <c r="B5" s="6">
@@ -2229,26 +2269,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="19.5" customHeight="1">
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
-      <c r="I5" s="52" t="s">
+      <c r="I5" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="J5" s="53"/>
-      <c r="K5" s="54"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="61"/>
     </row>
     <row r="6" spans="2:12" ht="32.25" customHeight="1">
       <c r="B6" s="10" t="s">
@@ -2269,9 +2309,9 @@
       <c r="G6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="57"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="64"/>
     </row>
     <row r="7" spans="2:12" ht="25.5">
       <c r="B7" s="4">
@@ -2292,9 +2332,9 @@
       <c r="G7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="57"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="64"/>
     </row>
     <row r="8" spans="2:12" ht="25.5">
       <c r="B8" s="4">
@@ -2315,9 +2355,9 @@
       <c r="G8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="55"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="57"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="64"/>
     </row>
     <row r="9" spans="2:12" ht="25.5">
       <c r="B9" s="4">
@@ -2338,9 +2378,9 @@
       <c r="G9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="58"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="60"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="67"/>
     </row>
     <row r="10" spans="2:12" ht="25.5">
       <c r="B10" s="4">
@@ -2401,12 +2441,12 @@
       <c r="G12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="51" t="s">
+      <c r="I12" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
     </row>
     <row r="13" spans="2:12" ht="25.5">
       <c r="B13" s="4">
@@ -2427,10 +2467,10 @@
       <c r="G13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
     </row>
     <row r="14" spans="2:12" ht="25.5">
       <c r="B14" s="4">
@@ -2589,11 +2629,11 @@
       <c r="G22" s="19"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -3139,10 +3179,10 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B54" s="50" t="s">
+      <c r="B54" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="50"/>
+      <c r="C54" s="57"/>
     </row>
     <row r="55" spans="2:7" ht="25.5">
       <c r="B55" s="22" t="s">
@@ -3365,11 +3405,11 @@
       </c>
     </row>
     <row r="69" spans="2:7" ht="15.75">
-      <c r="B69" s="50" t="s">
+      <c r="B69" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="C69" s="50"/>
-      <c r="D69" s="50"/>
+      <c r="C69" s="57"/>
+      <c r="D69" s="57"/>
     </row>
     <row r="70" spans="2:7" ht="25.5">
       <c r="B70" s="22" t="s">
@@ -3805,13 +3845,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" customHeight="1">
       <c r="B2" s="12"/>
@@ -3819,43 +3859,43 @@
       <c r="D2" s="25"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="54"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="61"/>
     </row>
     <row r="3" spans="1:15" ht="15.75">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="60"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="67"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
     </row>
     <row r="6" spans="1:15" ht="51.75" customHeight="1">
       <c r="A6" s="10" t="s">
@@ -4186,14 +4226,14 @@
       <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="62" t="s">
+      <c r="A23" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
     </row>
     <row r="24" spans="1:6" ht="51">
       <c r="A24" s="10" t="s">
@@ -4452,14 +4492,14 @@
       <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="64"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="65"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="72"/>
     </row>
     <row r="39" spans="1:6" ht="38.25">
       <c r="A39" s="10" t="s">
@@ -4591,13 +4631,13 @@
     </row>
     <row r="46" spans="1:6" ht="24.95" customHeight="1">
       <c r="A46" s="2"/>
-      <c r="B46" s="63" t="s">
+      <c r="B46" s="70" t="s">
         <v>184</v>
       </c>
-      <c r="C46" s="64"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="64"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="71"/>
     </row>
     <row r="47" spans="1:6" ht="38.25">
       <c r="A47" s="10" t="s">
@@ -4738,7 +4778,7 @@
   <dimension ref="B2:P58"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4753,13 +4793,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="19.5">
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
     </row>
     <row r="3" spans="2:16" ht="19.5">
       <c r="C3" s="13"/>
@@ -4769,40 +4809,40 @@
       <c r="G3" s="13"/>
     </row>
     <row r="4" spans="2:16" ht="15.75">
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="76" t="s">
         <v>269</v>
       </c>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
     </row>
     <row r="5" spans="2:16">
-      <c r="I5" s="52" t="s">
+      <c r="I5" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="54"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="61"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="60"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="67"/>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" s="10" t="s">
@@ -5021,11 +5061,11 @@
       </c>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="75"/>
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="10" t="s">
@@ -5299,11 +5339,11 @@
       <c r="C34" s="32"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
     </row>
     <row r="38" spans="2:7">
       <c r="B38" s="10" t="s">
@@ -5554,11 +5594,11 @@
       <c r="G50" s="1"/>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="68" t="s">
+      <c r="B53" s="75" t="s">
         <v>184</v>
       </c>
-      <c r="C53" s="68"/>
-      <c r="D53" s="68"/>
+      <c r="C53" s="75"/>
+      <c r="D53" s="75"/>
     </row>
     <row r="54" spans="2:7">
       <c r="B54" s="10" t="s">
@@ -5684,13 +5724,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:15" ht="19.5">
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
     </row>
     <row r="3" spans="3:15" ht="19.5">
       <c r="D3" s="13"/>
@@ -5698,45 +5738,45 @@
       <c r="F3" s="25"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="J3" s="70" t="s">
+      <c r="J3" s="77" t="s">
         <v>314</v>
       </c>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
     </row>
     <row r="4" spans="3:15" ht="15.75">
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="76" t="s">
         <v>306</v>
       </c>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
     </row>
     <row r="5" spans="3:15">
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
     </row>
     <row r="6" spans="3:15">
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="70"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
     </row>
     <row r="7" spans="3:15" ht="24" customHeight="1">
       <c r="C7" s="10" t="s">
@@ -6692,8 +6732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6705,143 +6745,230 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" ht="39.75" customHeight="1">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="71" t="s">
+      <c r="C4" s="48" t="s">
         <v>328</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="E4" s="71" t="s">
+      <c r="E4" s="48" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="62.25" customHeight="1">
-      <c r="B5" s="72">
+      <c r="B5" s="49">
         <v>1</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="50" t="s">
         <v>335</v>
       </c>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="51" t="s">
         <v>337</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="54" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="30">
-      <c r="B6" s="72">
+      <c r="B6" s="49">
         <v>2</v>
       </c>
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="53" t="s">
         <v>331</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="54" t="s">
         <v>347</v>
       </c>
-      <c r="E6" s="77" t="s">
+      <c r="E6" s="54" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="45">
-      <c r="B7" s="75">
+      <c r="B7" s="52">
         <v>3</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="52" t="s">
         <v>330</v>
       </c>
-      <c r="D7" s="77" t="s">
+      <c r="D7" s="54" t="s">
         <v>346</v>
       </c>
-      <c r="E7" s="77" t="s">
+      <c r="E7" s="54" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="60">
-      <c r="B8" s="75">
+      <c r="B8" s="52">
         <v>4</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="54" t="s">
         <v>341</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="54" t="s">
         <v>342</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="54" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="75">
-      <c r="B9" s="75">
+      <c r="B9" s="52">
         <v>5</v>
       </c>
-      <c r="C9" s="75" t="s">
+      <c r="C9" s="52" t="s">
         <v>336</v>
       </c>
-      <c r="D9" s="77" t="s">
+      <c r="D9" s="54" t="s">
         <v>345</v>
       </c>
-      <c r="E9" s="77" t="s">
+      <c r="E9" s="54" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="60">
-      <c r="B10" s="75">
+    <row r="10" spans="2:5" ht="45">
+      <c r="B10" s="52">
         <v>6</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="52" t="s">
         <v>329</v>
       </c>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="54" t="s">
         <v>344</v>
       </c>
-      <c r="E10" s="77" t="s">
+      <c r="E10" s="54" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="49.5" customHeight="1">
-      <c r="B11" s="75">
+      <c r="B11" s="52">
         <v>7</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="53" t="s">
         <v>332</v>
       </c>
-      <c r="D11" s="77" t="s">
+      <c r="D11" s="54" t="s">
         <v>351</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="E11" s="54" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="49.5" customHeight="1">
-      <c r="B12" s="75">
+      <c r="B12" s="52">
         <v>8</v>
       </c>
-      <c r="C12" s="77" t="s">
+      <c r="C12" s="54" t="s">
         <v>333</v>
       </c>
-      <c r="D12" s="77" t="s">
+      <c r="D12" s="54" t="s">
         <v>353</v>
       </c>
-      <c r="E12" s="77" t="s">
+      <c r="E12" s="54" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="30">
-      <c r="B13" s="75">
+      <c r="B13" s="52">
         <v>9</v>
       </c>
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="53" t="s">
         <v>334</v>
       </c>
-      <c r="D13" s="77" t="s">
+      <c r="D13" s="54" t="s">
         <v>354</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="54" t="s">
         <v>350</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C4:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="5.42578125" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" customWidth="1"/>
+    <col min="5" max="5" width="82.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" ht="25.5" customHeight="1">
+      <c r="C4" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>355</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="45">
+      <c r="C5" s="52">
+        <v>1</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>357</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="75">
+      <c r="C6" s="52">
+        <v>2</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>356</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" ht="30">
+      <c r="C7" s="52">
+        <v>3</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>358</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="60">
+      <c r="C8" s="52">
+        <v>4</v>
+      </c>
+      <c r="D8" s="54" t="s">
+        <v>359</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="45">
+      <c r="C9" s="52">
+        <v>6</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>360</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SAR Filling done and data after filling sar commited and pushed
</commit_message>
<xml_diff>
--- a/C2/C2 NBA All Tables Conso.xlsx
+++ b/C2/C2 NBA All Tables Conso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Personality develop. cell" sheetId="4" r:id="rId1"/>
@@ -2061,84 +2061,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2156,19 +2078,97 @@
     </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2442,7 +2442,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2465,21 +2465,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="H3" s="67" t="s">
+      <c r="H3" s="75" t="s">
         <v>185</v>
       </c>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
     </row>
     <row r="4" spans="2:12" ht="15.75">
       <c r="B4" s="45" t="s">
@@ -2497,11 +2497,11 @@
       <c r="F4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
     </row>
     <row r="5" spans="2:12" ht="31.5">
       <c r="B5" s="46">
@@ -2633,26 +2633,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="19.5" customHeight="1">
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
-      <c r="I5" s="70" t="s">
+      <c r="I5" s="78" t="s">
         <v>130</v>
       </c>
-      <c r="J5" s="71"/>
-      <c r="K5" s="72"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="80"/>
     </row>
     <row r="6" spans="2:12" ht="32.25" customHeight="1">
       <c r="B6" s="6" t="s">
@@ -2673,9 +2673,9 @@
       <c r="G6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="75"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="83"/>
     </row>
     <row r="7" spans="2:12" ht="25.5">
       <c r="B7" s="3">
@@ -2696,9 +2696,9 @@
       <c r="G7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="75"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="83"/>
     </row>
     <row r="8" spans="2:12" ht="25.5">
       <c r="B8" s="3">
@@ -2719,9 +2719,9 @@
       <c r="G8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="73"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="75"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="83"/>
     </row>
     <row r="9" spans="2:12" ht="25.5">
       <c r="B9" s="3">
@@ -2742,9 +2742,9 @@
       <c r="G9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="76"/>
-      <c r="J9" s="77"/>
-      <c r="K9" s="78"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="86"/>
     </row>
     <row r="10" spans="2:12" ht="25.5">
       <c r="B10" s="3">
@@ -2805,12 +2805,12 @@
       <c r="G12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="69" t="s">
+      <c r="I12" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="77"/>
+      <c r="L12" s="77"/>
     </row>
     <row r="13" spans="2:12" ht="25.5">
       <c r="B13" s="3">
@@ -2831,10 +2831,10 @@
       <c r="G13" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="69"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="77"/>
+      <c r="K13" s="77"/>
+      <c r="L13" s="77"/>
     </row>
     <row r="14" spans="2:12" ht="25.5">
       <c r="B14" s="3">
@@ -2993,11 +2993,11 @@
       <c r="G22" s="14"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="80" t="s">
+      <c r="B24" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
@@ -3543,10 +3543,10 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B54" s="68" t="s">
+      <c r="B54" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="C54" s="68"/>
+      <c r="C54" s="76"/>
     </row>
     <row r="55" spans="2:7" ht="25.5">
       <c r="B55" s="17" t="s">
@@ -3769,11 +3769,11 @@
       </c>
     </row>
     <row r="69" spans="2:7" ht="15.75">
-      <c r="B69" s="68" t="s">
+      <c r="B69" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="C69" s="68"/>
-      <c r="D69" s="68"/>
+      <c r="C69" s="76"/>
+      <c r="D69" s="76"/>
     </row>
     <row r="70" spans="2:7" ht="25.5">
       <c r="B70" s="17" t="s">
@@ -4194,7 +4194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
@@ -4210,13 +4210,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" customHeight="1">
       <c r="B2" s="49"/>
@@ -4224,39 +4224,39 @@
       <c r="D2" s="50"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="90" t="s">
         <v>184</v>
       </c>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="83"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="96" t="s">
         <v>365</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="86"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="94"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="95"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="88"/>
+      <c r="B5" s="89"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51"/>
       <c r="E5" s="51"/>
@@ -4591,10 +4591,10 @@
       <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="88" t="s">
+      <c r="A23" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="88"/>
+      <c r="B23" s="89"/>
       <c r="C23" s="51"/>
       <c r="D23" s="51"/>
       <c r="E23" s="51"/>
@@ -4837,10 +4837,10 @@
       <c r="F36" s="63"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="88" t="s">
+      <c r="A37" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="88"/>
+      <c r="B37" s="89"/>
       <c r="C37" s="51"/>
       <c r="D37" s="51"/>
       <c r="E37" s="51"/>
@@ -4975,10 +4975,10 @@
       <c r="F44" s="63"/>
     </row>
     <row r="45" spans="1:6" ht="21" customHeight="1">
-      <c r="A45" s="88" t="s">
+      <c r="A45" s="89" t="s">
         <v>182</v>
       </c>
-      <c r="B45" s="88"/>
+      <c r="B45" s="89"/>
       <c r="C45" s="51"/>
       <c r="D45" s="51"/>
       <c r="E45" s="51"/>
@@ -5123,7 +5123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:P58"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:G8"/>
     </sheetView>
   </sheetViews>
@@ -5139,13 +5139,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="19.5">
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
     </row>
     <row r="3" spans="2:16" ht="19.5">
       <c r="C3" s="8"/>
@@ -5155,40 +5155,40 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="2:16" ht="15.75">
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="98" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
     </row>
     <row r="5" spans="2:16">
-      <c r="I5" s="70" t="s">
+      <c r="I5" s="78" t="s">
         <v>184</v>
       </c>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="72"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="80"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="78"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="86"/>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" s="6" t="s">
@@ -5407,11 +5407,11 @@
       </c>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="89" t="s">
+      <c r="B19" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="89"/>
-      <c r="D19" s="89"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="97"/>
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="6" t="s">
@@ -5685,11 +5685,11 @@
       <c r="C34" s="21"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="89" t="s">
+      <c r="B37" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="89"/>
-      <c r="D37" s="89"/>
+      <c r="C37" s="97"/>
+      <c r="D37" s="97"/>
     </row>
     <row r="38" spans="2:7">
       <c r="B38" s="6" t="s">
@@ -5940,11 +5940,11 @@
       <c r="G50" s="1"/>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="89" t="s">
+      <c r="B53" s="97" t="s">
         <v>182</v>
       </c>
-      <c r="C53" s="89"/>
-      <c r="D53" s="89"/>
+      <c r="C53" s="97"/>
+      <c r="D53" s="97"/>
     </row>
     <row r="54" spans="2:7">
       <c r="B54" s="6" t="s">
@@ -6055,7 +6055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:P57"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C36" sqref="C36:H57"/>
     </sheetView>
   </sheetViews>
@@ -6070,13 +6070,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:15" ht="19.5">
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
     </row>
     <row r="3" spans="3:15" ht="19.5">
       <c r="D3" s="8"/>
@@ -6084,45 +6084,45 @@
       <c r="F3" s="20"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="J3" s="91" t="s">
+      <c r="J3" s="99" t="s">
         <v>312</v>
       </c>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
     </row>
     <row r="4" spans="3:15" ht="15.75">
-      <c r="D4" s="90" t="s">
+      <c r="D4" s="98" t="s">
         <v>304</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="91"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="99"/>
     </row>
     <row r="5" spans="3:15">
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="91"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="99"/>
+      <c r="N5" s="99"/>
+      <c r="O5" s="99"/>
     </row>
     <row r="6" spans="3:15">
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="91"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="99"/>
     </row>
     <row r="7" spans="3:15" ht="24" customHeight="1">
       <c r="C7" s="6" t="s">
@@ -7327,183 +7327,183 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C22" sqref="C22:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="101"/>
-    <col min="3" max="3" width="75.5703125" style="101" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" style="101" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="101" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="101" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37" style="101" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" style="101" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="101"/>
+    <col min="1" max="2" width="9.140625" style="72"/>
+    <col min="3" max="3" width="75.5703125" style="72" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" style="72" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="72" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" style="72" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37" style="72" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="72" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="72"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="102" t="s">
         <v>400</v>
       </c>
-      <c r="C3" s="100"/>
+      <c r="C3" s="102"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="66" t="s">
         <v>376</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="66" t="s">
         <v>377</v>
       </c>
-      <c r="D4" s="92" t="s">
+      <c r="D4" s="66" t="s">
         <v>378</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="66" t="s">
         <v>379</v>
       </c>
-      <c r="F4" s="92" t="s">
+      <c r="F4" s="66" t="s">
         <v>380</v>
       </c>
-      <c r="G4" s="92" t="s">
+      <c r="G4" s="66" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="21.75" customHeight="1">
-      <c r="B5" s="93">
+      <c r="B5" s="67">
         <v>1</v>
       </c>
-      <c r="C5" s="94" t="s">
+      <c r="C5" s="68" t="s">
         <v>382</v>
       </c>
-      <c r="D5" s="94" t="s">
+      <c r="D5" s="68" t="s">
         <v>383</v>
       </c>
-      <c r="E5" s="95"/>
-      <c r="F5" s="94" t="s">
+      <c r="E5" s="69"/>
+      <c r="F5" s="68" t="s">
         <v>384</v>
       </c>
-      <c r="G5" s="96" t="s">
+      <c r="G5" s="70" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="31.5">
-      <c r="B6" s="93">
+      <c r="B6" s="67">
         <v>2</v>
       </c>
-      <c r="C6" s="94" t="s">
+      <c r="C6" s="68" t="s">
         <v>397</v>
       </c>
-      <c r="D6" s="94" t="s">
+      <c r="D6" s="68" t="s">
         <v>398</v>
       </c>
-      <c r="E6" s="95"/>
-      <c r="F6" s="96" t="s">
+      <c r="E6" s="69"/>
+      <c r="F6" s="70" t="s">
         <v>386</v>
       </c>
-      <c r="G6" s="96" t="s">
+      <c r="G6" s="70" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="102">
+      <c r="B7" s="73">
         <v>3</v>
       </c>
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="68" t="s">
         <v>388</v>
       </c>
-      <c r="D7" s="94" t="s">
+      <c r="D7" s="68" t="s">
         <v>389</v>
       </c>
-      <c r="E7" s="96" t="s">
+      <c r="E7" s="70" t="s">
         <v>390</v>
       </c>
-      <c r="F7" s="94" t="s">
+      <c r="F7" s="68" t="s">
         <v>391</v>
       </c>
-      <c r="G7" s="96" t="s">
+      <c r="G7" s="70" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="93">
+      <c r="B8" s="67">
         <v>4</v>
       </c>
-      <c r="C8" s="94" t="s">
+      <c r="C8" s="68" t="s">
         <v>393</v>
       </c>
-      <c r="D8" s="94" t="s">
+      <c r="D8" s="68" t="s">
         <v>394</v>
       </c>
-      <c r="E8" s="96" t="s">
+      <c r="E8" s="70" t="s">
         <v>390</v>
       </c>
-      <c r="F8" s="94" t="s">
+      <c r="F8" s="68" t="s">
         <v>391</v>
       </c>
-      <c r="G8" s="96" t="s">
+      <c r="G8" s="70" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="93">
+      <c r="B9" s="67">
         <v>5</v>
       </c>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="68" t="s">
         <v>395</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="68" t="s">
         <v>399</v>
       </c>
-      <c r="E9" s="95"/>
-      <c r="F9" s="94" t="s">
+      <c r="E9" s="69"/>
+      <c r="F9" s="68" t="s">
         <v>396</v>
       </c>
-      <c r="G9" s="96" t="s">
+      <c r="G9" s="70" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="100" t="s">
+      <c r="B12" s="102" t="s">
         <v>400</v>
       </c>
-      <c r="C12" s="100"/>
+      <c r="C12" s="102"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="66" t="s">
         <v>376</v>
       </c>
-      <c r="C13" s="92" t="s">
+      <c r="C13" s="66" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="92" t="s">
+      <c r="D13" s="66" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="92" t="s">
+      <c r="E13" s="66" t="s">
         <v>379</v>
       </c>
-      <c r="F13" s="92" t="s">
+      <c r="F13" s="66" t="s">
         <v>380</v>
       </c>
-      <c r="G13" s="92" t="s">
+      <c r="G13" s="66" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="93">
+      <c r="B14" s="67">
         <v>1</v>
       </c>
-      <c r="C14" s="94" t="s">
+      <c r="C14" s="68" t="s">
         <v>382</v>
       </c>
-      <c r="D14" s="94" t="s">
+      <c r="D14" s="68" t="s">
         <v>383</v>
       </c>
-      <c r="E14" s="95"/>
-      <c r="F14" s="94" t="s">
+      <c r="E14" s="69"/>
+      <c r="F14" s="68" t="s">
         <v>384</v>
       </c>
-      <c r="G14" s="96" t="s">
+      <c r="G14" s="70" t="s">
         <v>385</v>
       </c>
     </row>
@@ -7543,7 +7543,7 @@
       <c r="E18" s="38" t="s">
         <v>404</v>
       </c>
-      <c r="F18" s="97">
+      <c r="F18" s="71">
         <v>43276</v>
       </c>
       <c r="G18" s="38" t="s">
@@ -7566,7 +7566,7 @@
       <c r="E19" s="38" t="s">
         <v>407</v>
       </c>
-      <c r="F19" s="97">
+      <c r="F19" s="71">
         <v>43307</v>
       </c>
       <c r="G19" s="38" t="s">
@@ -7577,72 +7577,72 @@
       </c>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="98">
+      <c r="B20" s="100">
         <v>3</v>
       </c>
-      <c r="C20" s="98" t="s">
+      <c r="C20" s="100" t="s">
         <v>410</v>
       </c>
-      <c r="D20" s="98" t="s">
+      <c r="D20" s="100" t="s">
         <v>411</v>
       </c>
-      <c r="E20" s="98" t="s">
+      <c r="E20" s="100" t="s">
         <v>412</v>
       </c>
-      <c r="F20" s="97">
+      <c r="F20" s="71">
         <v>43344</v>
       </c>
-      <c r="G20" s="98" t="s">
+      <c r="G20" s="100" t="s">
         <v>405</v>
       </c>
-      <c r="H20" s="98" t="s">
+      <c r="H20" s="100" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="98"/>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="97">
+      <c r="B21" s="100"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="71">
         <v>43345</v>
       </c>
-      <c r="G21" s="98"/>
-      <c r="H21" s="98"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="100"/>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="98">
+      <c r="B22" s="100">
         <v>4</v>
       </c>
-      <c r="C22" s="98" t="s">
+      <c r="C22" s="100" t="s">
         <v>414</v>
       </c>
-      <c r="D22" s="98" t="s">
+      <c r="D22" s="100" t="s">
         <v>415</v>
       </c>
-      <c r="E22" s="98" t="s">
+      <c r="E22" s="100" t="s">
         <v>416</v>
       </c>
-      <c r="F22" s="99">
+      <c r="F22" s="101">
         <v>43473</v>
       </c>
       <c r="G22" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="H22" s="98" t="s">
+      <c r="H22" s="100" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="98"/>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98"/>
+      <c r="B23" s="100"/>
+      <c r="C23" s="100"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="100"/>
+      <c r="F23" s="100"/>
       <c r="G23" s="38" t="s">
         <v>418</v>
       </c>
-      <c r="H23" s="98"/>
+      <c r="H23" s="100"/>
     </row>
     <row r="24" spans="2:8" ht="110.25">
       <c r="B24" s="38">
@@ -7657,7 +7657,7 @@
       <c r="E24" s="38" t="s">
         <v>421</v>
       </c>
-      <c r="F24" s="97">
+      <c r="F24" s="71">
         <v>43473</v>
       </c>
       <c r="G24" s="38" t="s">
@@ -7688,90 +7688,90 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="98">
+      <c r="B30" s="100">
         <v>1</v>
       </c>
-      <c r="C30" s="98" t="s">
+      <c r="C30" s="100" t="s">
         <v>427</v>
       </c>
-      <c r="D30" s="98" t="s">
+      <c r="D30" s="100" t="s">
         <v>366</v>
       </c>
-      <c r="E30" s="98" t="s">
+      <c r="E30" s="100" t="s">
         <v>428</v>
       </c>
       <c r="F30" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="G30" s="98" t="s">
+      <c r="G30" s="100" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="98"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="98"/>
+      <c r="B31" s="100"/>
+      <c r="C31" s="100"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="100"/>
       <c r="F31" s="38" t="s">
         <v>429</v>
       </c>
-      <c r="G31" s="98"/>
+      <c r="G31" s="100"/>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="98">
+      <c r="B32" s="100">
         <v>2</v>
       </c>
-      <c r="C32" s="98" t="s">
+      <c r="C32" s="100" t="s">
         <v>430</v>
       </c>
-      <c r="D32" s="98" t="s">
+      <c r="D32" s="100" t="s">
         <v>367</v>
       </c>
-      <c r="E32" s="98" t="s">
+      <c r="E32" s="100" t="s">
         <v>431</v>
       </c>
-      <c r="F32" s="98" t="s">
+      <c r="F32" s="100" t="s">
         <v>405</v>
       </c>
-      <c r="G32" s="98" t="s">
+      <c r="G32" s="100" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="98"/>
-      <c r="C33" s="98"/>
-      <c r="D33" s="98"/>
-      <c r="E33" s="98"/>
-      <c r="F33" s="98"/>
-      <c r="G33" s="98"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="100"/>
+      <c r="D33" s="100"/>
+      <c r="E33" s="100"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="100"/>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="98">
+      <c r="B34" s="100">
         <v>3</v>
       </c>
-      <c r="C34" s="98" t="s">
+      <c r="C34" s="100" t="s">
         <v>433</v>
       </c>
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="100" t="s">
         <v>368</v>
       </c>
-      <c r="E34" s="98" t="s">
+      <c r="E34" s="100" t="s">
         <v>434</v>
       </c>
-      <c r="F34" s="98" t="s">
+      <c r="F34" s="100" t="s">
         <v>405</v>
       </c>
-      <c r="G34" s="98" t="s">
+      <c r="G34" s="100" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="98"/>
-      <c r="C35" s="98"/>
-      <c r="D35" s="98"/>
-      <c r="E35" s="98"/>
-      <c r="F35" s="98"/>
-      <c r="G35" s="98"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="100"/>
+      <c r="D35" s="100"/>
+      <c r="E35" s="100"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="100"/>
     </row>
     <row r="36" spans="2:7" ht="31.5">
       <c r="B36" s="38">
@@ -7814,10 +7814,10 @@
       </c>
     </row>
     <row r="42" spans="2:7" ht="31.5">
-      <c r="B42" s="98">
+      <c r="B42" s="100">
         <v>1</v>
       </c>
-      <c r="C42" s="98" t="s">
+      <c r="C42" s="100" t="s">
         <v>427</v>
       </c>
       <c r="D42" s="38" t="s">
@@ -7829,13 +7829,13 @@
       <c r="F42" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="G42" s="98" t="s">
+      <c r="G42" s="100" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="47.25">
-      <c r="B43" s="98"/>
-      <c r="C43" s="98"/>
+      <c r="B43" s="100"/>
+      <c r="C43" s="100"/>
       <c r="D43" s="38" t="s">
         <v>439</v>
       </c>
@@ -7845,16 +7845,16 @@
       <c r="F43" s="38" t="s">
         <v>429</v>
       </c>
-      <c r="G43" s="98"/>
+      <c r="G43" s="100"/>
     </row>
     <row r="44" spans="2:7" ht="31.5">
-      <c r="B44" s="98">
+      <c r="B44" s="100">
         <v>2</v>
       </c>
-      <c r="C44" s="98" t="s">
+      <c r="C44" s="100" t="s">
         <v>441</v>
       </c>
-      <c r="D44" s="98" t="s">
+      <c r="D44" s="100" t="s">
         <v>442</v>
       </c>
       <c r="E44" s="38" t="s">
@@ -7863,51 +7863,51 @@
       <c r="F44" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="G44" s="98" t="s">
+      <c r="G44" s="100" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="31.5">
-      <c r="B45" s="98"/>
-      <c r="C45" s="98"/>
-      <c r="D45" s="98"/>
+      <c r="B45" s="100"/>
+      <c r="C45" s="100"/>
+      <c r="D45" s="100"/>
       <c r="E45" s="38" t="s">
         <v>444</v>
       </c>
       <c r="F45" s="38" t="s">
         <v>429</v>
       </c>
-      <c r="G45" s="98"/>
+      <c r="G45" s="100"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="98">
+      <c r="B46" s="100">
         <v>3</v>
       </c>
-      <c r="C46" s="98" t="s">
+      <c r="C46" s="100" t="s">
         <v>445</v>
       </c>
-      <c r="D46" s="98" t="s">
+      <c r="D46" s="100" t="s">
         <v>446</v>
       </c>
-      <c r="E46" s="98" t="s">
+      <c r="E46" s="100" t="s">
         <v>447</v>
       </c>
       <c r="F46" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="G46" s="98" t="s">
+      <c r="G46" s="100" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="47" spans="2:7">
-      <c r="B47" s="98"/>
-      <c r="C47" s="98"/>
-      <c r="D47" s="98"/>
-      <c r="E47" s="98"/>
+      <c r="B47" s="100"/>
+      <c r="C47" s="100"/>
+      <c r="D47" s="100"/>
+      <c r="E47" s="100"/>
       <c r="F47" s="38" t="s">
         <v>449</v>
       </c>
-      <c r="G47" s="98"/>
+      <c r="G47" s="100"/>
     </row>
     <row r="48" spans="2:7" ht="31.5">
       <c r="B48" s="38">
@@ -7931,11 +7931,37 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="G42:G43"/>
@@ -7943,37 +7969,11 @@
     <mergeCell ref="C44:C45"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="G44:G45"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="G46:G47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
C2 IV-asp and WK/Exprt lect RDK added
</commit_message>
<xml_diff>
--- a/C2/C2 NBA All Tables Conso.xlsx
+++ b/C2/C2 NBA All Tables Conso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Personality develop. cell" sheetId="4" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="2.2.6 A" sheetId="11" r:id="rId6"/>
     <sheet name="2.2.6 B" sheetId="12" r:id="rId7"/>
     <sheet name="IV and WK" sheetId="13" r:id="rId8"/>
+    <sheet name="IV ASP" sheetId="14" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="508">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -1488,6 +1489,171 @@
   <si>
     <t xml:space="preserve">Mr. Menkudale     Mr. Avinash Jadhav   Mrs. Varsha Swami </t>
   </si>
+  <si>
+    <t xml:space="preserve">Name Of Industry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address -Contact Details </t>
+  </si>
+  <si>
+    <t>Subject  Name</t>
+  </si>
+  <si>
+    <t>Name Of Staff to be involved</t>
+  </si>
+  <si>
+    <t>BSNL Office Gandhi Chowk, Latur-413512</t>
+  </si>
+  <si>
+    <t>CO3I</t>
+  </si>
+  <si>
+    <t>Mrs.A.S.Patil,                                   Mrs P.S.Bhujange</t>
+  </si>
+  <si>
+    <t>MIDC Area,Hadco Latur-413531</t>
+  </si>
+  <si>
+    <t>CPH-22013</t>
+  </si>
+  <si>
+    <t>CO2I</t>
+  </si>
+  <si>
+    <t>Mrs.A.S.Patil,                      Mr. R.S. Devkar</t>
+  </si>
+  <si>
+    <t>Operand Technology &amp; IT  Solutions Pvt.Ltd, Latur  (15/2/2020)</t>
+  </si>
+  <si>
+    <t>Barshi Road, near Cilai World Shop,Latur-413512</t>
+  </si>
+  <si>
+    <t>MAD- 22617</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CO6I</t>
+  </si>
+  <si>
+    <t>Mrs.A.S.Patil,                       Mr. S V. Chavan</t>
+  </si>
+  <si>
+    <t>Academic Year 2019-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSNL-Bharat Sanchar Nigam Limited Latur                      </t>
+  </si>
+  <si>
+    <t>Industrial Visit [IPR]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Arty Offset Industry,Latur            </t>
+  </si>
+  <si>
+    <t>CGR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print Pack Business Forms Pvt.Ltd  </t>
+  </si>
+  <si>
+    <t>16-MIDC Area,Latur-413512</t>
+  </si>
+  <si>
+    <t>WPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CO2I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mr. S V. Chavan  Ms.V.D.Dhere</t>
+  </si>
+  <si>
+    <t>BSNL-Bharat Sanchar Nigam Limited Latur     (8/8/2019)</t>
+  </si>
+  <si>
+    <t>Ms.R.D Kasar  Mr. S.D.Gheware</t>
+  </si>
+  <si>
+    <t>Ms.R.D Kasar     Mr.r.B.Salunke, Ms.V.D.Dhere</t>
+  </si>
+  <si>
+    <t>Academic Year 2018-19</t>
+  </si>
+  <si>
+    <t>Name of Industry</t>
+  </si>
+  <si>
+    <t>Address Contact Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semester </t>
+  </si>
+  <si>
+    <t>Subject Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of Staff to be involved </t>
+  </si>
+  <si>
+    <t>BSNL - Bharat Sanchar Nigam Limited Latur (08/09/2017)</t>
+  </si>
+  <si>
+    <t>BSNL office, Gandhi Chowk Latur- 413512</t>
+  </si>
+  <si>
+    <t>PPT</t>
+  </si>
+  <si>
+    <t>Mindlabz Software Solutions Latur (18/09/2017)</t>
+  </si>
+  <si>
+    <t>Behind Hotel Grand, Latur</t>
+  </si>
+  <si>
+    <t>Mrs. A. S Patil, Ms.Pathan A.S.</t>
+  </si>
+  <si>
+    <t>Mindlabz Software Solutions Latur   (09/10/2017)</t>
+  </si>
+  <si>
+    <t>Academic Year 2017-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. R D Kasar,  Mr. R B Salunke ,   Ms. A J Shashtri </t>
+  </si>
+  <si>
+    <t>Mr. S.V.Chavan, Mrs. A. S Patil</t>
+  </si>
+  <si>
+    <t>BSNL - Bharat Sanchar Nigam Limited Latur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. R D Kasar, Mr. R B Salunke , Ms. A J Shashtri </t>
+  </si>
+  <si>
+    <t>Arty offset industries Latur</t>
+  </si>
+  <si>
+    <t>MIDC area, Hadco Latur - 413531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs. A. S Patil, Mr. A R. Dharmadhikari </t>
+  </si>
+  <si>
+    <t>Oriange IT Services Pvt. Ltd. Latur</t>
+  </si>
+  <si>
+    <t>Near Water Tank, Barshi Road Latur - 413531</t>
+  </si>
+  <si>
+    <t>Ms. R D Kasar, Mrs. A S Patil</t>
+  </si>
+  <si>
+    <t>Academic Year 2016-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Arty Offset Industry,Latur  (7/2/2020)</t>
+  </si>
 </sst>
 </file>
 
@@ -1496,7 +1662,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1661,6 +1827,17 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1700,7 +1877,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1864,11 +2041,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2083,6 +2284,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2161,14 +2365,53 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2442,7 +2685,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2465,21 +2708,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="H3" s="75" t="s">
+      <c r="H3" s="76" t="s">
         <v>185</v>
       </c>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
     </row>
     <row r="4" spans="2:12" ht="15.75">
       <c r="B4" s="45" t="s">
@@ -2497,11 +2740,11 @@
       <c r="F4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
     </row>
     <row r="5" spans="2:12" ht="31.5">
       <c r="B5" s="46">
@@ -2633,26 +2876,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="19.5" customHeight="1">
-      <c r="D2" s="87" t="s">
+      <c r="D2" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
-      <c r="I5" s="78" t="s">
+      <c r="I5" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="J5" s="79"/>
-      <c r="K5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="81"/>
     </row>
     <row r="6" spans="2:12" ht="32.25" customHeight="1">
       <c r="B6" s="6" t="s">
@@ -2673,9 +2916,9 @@
       <c r="G6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="81"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="83"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="84"/>
     </row>
     <row r="7" spans="2:12" ht="25.5">
       <c r="B7" s="3">
@@ -2696,9 +2939,9 @@
       <c r="G7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="81"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="83"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="84"/>
     </row>
     <row r="8" spans="2:12" ht="25.5">
       <c r="B8" s="3">
@@ -2719,9 +2962,9 @@
       <c r="G8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="81"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="83"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="84"/>
     </row>
     <row r="9" spans="2:12" ht="25.5">
       <c r="B9" s="3">
@@ -2742,9 +2985,9 @@
       <c r="G9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="84"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="86"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="87"/>
     </row>
     <row r="10" spans="2:12" ht="25.5">
       <c r="B10" s="3">
@@ -2805,12 +3048,12 @@
       <c r="G12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="77" t="s">
+      <c r="I12" s="78" t="s">
         <v>129</v>
       </c>
-      <c r="J12" s="77"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="78"/>
     </row>
     <row r="13" spans="2:12" ht="25.5">
       <c r="B13" s="3">
@@ -2831,10 +3074,10 @@
       <c r="G13" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="77"/>
-      <c r="J13" s="77"/>
-      <c r="K13" s="77"/>
-      <c r="L13" s="77"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="78"/>
     </row>
     <row r="14" spans="2:12" ht="25.5">
       <c r="B14" s="3">
@@ -2993,11 +3236,11 @@
       <c r="G22" s="14"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="88" t="s">
+      <c r="B24" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
@@ -3543,10 +3786,10 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B54" s="76" t="s">
+      <c r="B54" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="C54" s="76"/>
+      <c r="C54" s="77"/>
     </row>
     <row r="55" spans="2:7" ht="25.5">
       <c r="B55" s="17" t="s">
@@ -3769,11 +4012,11 @@
       </c>
     </row>
     <row r="69" spans="2:7" ht="15.75">
-      <c r="B69" s="76" t="s">
+      <c r="B69" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="C69" s="76"/>
-      <c r="D69" s="76"/>
+      <c r="C69" s="77"/>
+      <c r="D69" s="77"/>
     </row>
     <row r="70" spans="2:7" ht="25.5">
       <c r="B70" s="17" t="s">
@@ -4194,7 +4437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
@@ -4210,13 +4453,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" customHeight="1">
       <c r="B2" s="49"/>
@@ -4224,39 +4467,39 @@
       <c r="D2" s="50"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
-      <c r="H2" s="90" t="s">
+      <c r="H2" s="91" t="s">
         <v>184</v>
       </c>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="93"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>365</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="95"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="96"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="89"/>
+      <c r="B5" s="90"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51"/>
       <c r="E5" s="51"/>
@@ -4591,10 +4834,10 @@
       <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="89" t="s">
+      <c r="A23" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="89"/>
+      <c r="B23" s="90"/>
       <c r="C23" s="51"/>
       <c r="D23" s="51"/>
       <c r="E23" s="51"/>
@@ -4837,10 +5080,10 @@
       <c r="F36" s="63"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="89" t="s">
+      <c r="A37" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="89"/>
+      <c r="B37" s="90"/>
       <c r="C37" s="51"/>
       <c r="D37" s="51"/>
       <c r="E37" s="51"/>
@@ -4975,10 +5218,10 @@
       <c r="F44" s="63"/>
     </row>
     <row r="45" spans="1:6" ht="21" customHeight="1">
-      <c r="A45" s="89" t="s">
+      <c r="A45" s="90" t="s">
         <v>182</v>
       </c>
-      <c r="B45" s="89"/>
+      <c r="B45" s="90"/>
       <c r="C45" s="51"/>
       <c r="D45" s="51"/>
       <c r="E45" s="51"/>
@@ -5139,13 +5382,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="19.5">
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
     </row>
     <row r="3" spans="2:16" ht="19.5">
       <c r="C3" s="8"/>
@@ -5155,40 +5398,40 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="2:16" ht="15.75">
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="99" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
     </row>
     <row r="5" spans="2:16">
-      <c r="I5" s="78" t="s">
+      <c r="I5" s="79" t="s">
         <v>184</v>
       </c>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="81"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="85"/>
-      <c r="M6" s="85"/>
-      <c r="N6" s="85"/>
-      <c r="O6" s="85"/>
-      <c r="P6" s="86"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="87"/>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" s="6" t="s">
@@ -5407,11 +5650,11 @@
       </c>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="97" t="s">
+      <c r="B19" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="97"/>
-      <c r="D19" s="97"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="98"/>
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="6" t="s">
@@ -5685,11 +5928,11 @@
       <c r="C34" s="21"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="97" t="s">
+      <c r="B37" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="97"/>
-      <c r="D37" s="97"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="98"/>
     </row>
     <row r="38" spans="2:7">
       <c r="B38" s="6" t="s">
@@ -5940,11 +6183,11 @@
       <c r="G50" s="1"/>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="97" t="s">
+      <c r="B53" s="98" t="s">
         <v>182</v>
       </c>
-      <c r="C53" s="97"/>
-      <c r="D53" s="97"/>
+      <c r="C53" s="98"/>
+      <c r="D53" s="98"/>
     </row>
     <row r="54" spans="2:7">
       <c r="B54" s="6" t="s">
@@ -6070,13 +6313,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:15" ht="19.5">
-      <c r="D2" s="87" t="s">
+      <c r="D2" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
     </row>
     <row r="3" spans="3:15" ht="19.5">
       <c r="D3" s="8"/>
@@ -6084,45 +6327,45 @@
       <c r="F3" s="20"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="J3" s="99" t="s">
+      <c r="J3" s="100" t="s">
         <v>312</v>
       </c>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
     </row>
     <row r="4" spans="3:15" ht="15.75">
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="99" t="s">
         <v>304</v>
       </c>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
-      <c r="N4" s="99"/>
-      <c r="O4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="100"/>
+      <c r="O4" s="100"/>
     </row>
     <row r="5" spans="3:15">
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
-      <c r="O5" s="99"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
+      <c r="N5" s="100"/>
+      <c r="O5" s="100"/>
     </row>
     <row r="6" spans="3:15">
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="99"/>
-      <c r="N6" s="99"/>
-      <c r="O6" s="99"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
+      <c r="N6" s="100"/>
+      <c r="O6" s="100"/>
     </row>
     <row r="7" spans="3:15" ht="24" customHeight="1">
       <c r="C7" s="6" t="s">
@@ -7327,7 +7570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:H48"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C22" sqref="C22:C23"/>
     </sheetView>
   </sheetViews>
@@ -7344,10 +7587,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="101" t="s">
         <v>400</v>
       </c>
-      <c r="C3" s="102"/>
+      <c r="C3" s="101"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="66" t="s">
@@ -7464,10 +7707,10 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="102" t="s">
+      <c r="B12" s="101" t="s">
         <v>400</v>
       </c>
-      <c r="C12" s="102"/>
+      <c r="C12" s="101"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="66" t="s">
@@ -7577,72 +7820,72 @@
       </c>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="100">
+      <c r="B20" s="102">
         <v>3</v>
       </c>
-      <c r="C20" s="100" t="s">
+      <c r="C20" s="102" t="s">
         <v>410</v>
       </c>
-      <c r="D20" s="100" t="s">
+      <c r="D20" s="102" t="s">
         <v>411</v>
       </c>
-      <c r="E20" s="100" t="s">
+      <c r="E20" s="102" t="s">
         <v>412</v>
       </c>
       <c r="F20" s="71">
         <v>43344</v>
       </c>
-      <c r="G20" s="100" t="s">
+      <c r="G20" s="102" t="s">
         <v>405</v>
       </c>
-      <c r="H20" s="100" t="s">
+      <c r="H20" s="102" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="100"/>
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
       <c r="F21" s="71">
         <v>43345</v>
       </c>
-      <c r="G21" s="100"/>
-      <c r="H21" s="100"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="102"/>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="100">
+      <c r="B22" s="102">
         <v>4</v>
       </c>
-      <c r="C22" s="100" t="s">
+      <c r="C22" s="102" t="s">
         <v>414</v>
       </c>
-      <c r="D22" s="100" t="s">
+      <c r="D22" s="102" t="s">
         <v>415</v>
       </c>
-      <c r="E22" s="100" t="s">
+      <c r="E22" s="102" t="s">
         <v>416</v>
       </c>
-      <c r="F22" s="101">
+      <c r="F22" s="103">
         <v>43473</v>
       </c>
       <c r="G22" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="H22" s="100" t="s">
+      <c r="H22" s="102" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="100"/>
-      <c r="C23" s="100"/>
-      <c r="D23" s="100"/>
-      <c r="E23" s="100"/>
-      <c r="F23" s="100"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="102"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
       <c r="G23" s="38" t="s">
         <v>418</v>
       </c>
-      <c r="H23" s="100"/>
+      <c r="H23" s="102"/>
     </row>
     <row r="24" spans="2:8" ht="110.25">
       <c r="B24" s="38">
@@ -7688,90 +7931,90 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="100">
+      <c r="B30" s="102">
         <v>1</v>
       </c>
-      <c r="C30" s="100" t="s">
+      <c r="C30" s="102" t="s">
         <v>427</v>
       </c>
-      <c r="D30" s="100" t="s">
+      <c r="D30" s="102" t="s">
         <v>366</v>
       </c>
-      <c r="E30" s="100" t="s">
+      <c r="E30" s="102" t="s">
         <v>428</v>
       </c>
       <c r="F30" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="G30" s="100" t="s">
+      <c r="G30" s="102" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="100"/>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="100"/>
+      <c r="B31" s="102"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="102"/>
       <c r="F31" s="38" t="s">
         <v>429</v>
       </c>
-      <c r="G31" s="100"/>
+      <c r="G31" s="102"/>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="100">
+      <c r="B32" s="102">
         <v>2</v>
       </c>
-      <c r="C32" s="100" t="s">
+      <c r="C32" s="102" t="s">
         <v>430</v>
       </c>
-      <c r="D32" s="100" t="s">
+      <c r="D32" s="102" t="s">
         <v>367</v>
       </c>
-      <c r="E32" s="100" t="s">
+      <c r="E32" s="102" t="s">
         <v>431</v>
       </c>
-      <c r="F32" s="100" t="s">
+      <c r="F32" s="102" t="s">
         <v>405</v>
       </c>
-      <c r="G32" s="100" t="s">
+      <c r="G32" s="102" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="100"/>
-      <c r="C33" s="100"/>
-      <c r="D33" s="100"/>
-      <c r="E33" s="100"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="100"/>
+      <c r="B33" s="102"/>
+      <c r="C33" s="102"/>
+      <c r="D33" s="102"/>
+      <c r="E33" s="102"/>
+      <c r="F33" s="102"/>
+      <c r="G33" s="102"/>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="100">
+      <c r="B34" s="102">
         <v>3</v>
       </c>
-      <c r="C34" s="100" t="s">
+      <c r="C34" s="102" t="s">
         <v>433</v>
       </c>
-      <c r="D34" s="100" t="s">
+      <c r="D34" s="102" t="s">
         <v>368</v>
       </c>
-      <c r="E34" s="100" t="s">
+      <c r="E34" s="102" t="s">
         <v>434</v>
       </c>
-      <c r="F34" s="100" t="s">
+      <c r="F34" s="102" t="s">
         <v>405</v>
       </c>
-      <c r="G34" s="100" t="s">
+      <c r="G34" s="102" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="100"/>
-      <c r="C35" s="100"/>
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="100"/>
+      <c r="B35" s="102"/>
+      <c r="C35" s="102"/>
+      <c r="D35" s="102"/>
+      <c r="E35" s="102"/>
+      <c r="F35" s="102"/>
+      <c r="G35" s="102"/>
     </row>
     <row r="36" spans="2:7" ht="31.5">
       <c r="B36" s="38">
@@ -7814,10 +8057,10 @@
       </c>
     </row>
     <row r="42" spans="2:7" ht="31.5">
-      <c r="B42" s="100">
+      <c r="B42" s="102">
         <v>1</v>
       </c>
-      <c r="C42" s="100" t="s">
+      <c r="C42" s="102" t="s">
         <v>427</v>
       </c>
       <c r="D42" s="38" t="s">
@@ -7829,13 +8072,13 @@
       <c r="F42" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="G42" s="100" t="s">
+      <c r="G42" s="102" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="47.25">
-      <c r="B43" s="100"/>
-      <c r="C43" s="100"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="102"/>
       <c r="D43" s="38" t="s">
         <v>439</v>
       </c>
@@ -7845,16 +8088,16 @@
       <c r="F43" s="38" t="s">
         <v>429</v>
       </c>
-      <c r="G43" s="100"/>
+      <c r="G43" s="102"/>
     </row>
     <row r="44" spans="2:7" ht="31.5">
-      <c r="B44" s="100">
+      <c r="B44" s="102">
         <v>2</v>
       </c>
-      <c r="C44" s="100" t="s">
+      <c r="C44" s="102" t="s">
         <v>441</v>
       </c>
-      <c r="D44" s="100" t="s">
+      <c r="D44" s="102" t="s">
         <v>442</v>
       </c>
       <c r="E44" s="38" t="s">
@@ -7863,51 +8106,51 @@
       <c r="F44" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="G44" s="100" t="s">
+      <c r="G44" s="102" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="31.5">
-      <c r="B45" s="100"/>
-      <c r="C45" s="100"/>
-      <c r="D45" s="100"/>
+      <c r="B45" s="102"/>
+      <c r="C45" s="102"/>
+      <c r="D45" s="102"/>
       <c r="E45" s="38" t="s">
         <v>444</v>
       </c>
       <c r="F45" s="38" t="s">
         <v>429</v>
       </c>
-      <c r="G45" s="100"/>
+      <c r="G45" s="102"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="100">
+      <c r="B46" s="102">
         <v>3</v>
       </c>
-      <c r="C46" s="100" t="s">
+      <c r="C46" s="102" t="s">
         <v>445</v>
       </c>
-      <c r="D46" s="100" t="s">
+      <c r="D46" s="102" t="s">
         <v>446</v>
       </c>
-      <c r="E46" s="100" t="s">
+      <c r="E46" s="102" t="s">
         <v>447</v>
       </c>
       <c r="F46" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="G46" s="100" t="s">
+      <c r="G46" s="102" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="47" spans="2:7">
-      <c r="B47" s="100"/>
-      <c r="C47" s="100"/>
-      <c r="D47" s="100"/>
-      <c r="E47" s="100"/>
+      <c r="B47" s="102"/>
+      <c r="C47" s="102"/>
+      <c r="D47" s="102"/>
+      <c r="E47" s="102"/>
       <c r="F47" s="38" t="s">
         <v>449</v>
       </c>
-      <c r="G47" s="100"/>
+      <c r="G47" s="102"/>
     </row>
     <row r="48" spans="2:7" ht="31.5">
       <c r="B48" s="38">
@@ -7931,6 +8174,35 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="G30:G31"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="H22:H23"/>
@@ -7945,35 +8217,387 @@
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="F22:F23"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="G46:G47"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" ht="15.75">
+      <c r="B3" s="114" t="s">
+        <v>469</v>
+      </c>
+      <c r="C3" s="115"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+    </row>
+    <row r="4" spans="2:7" ht="15.75">
+      <c r="B4" s="110" t="s">
+        <v>376</v>
+      </c>
+      <c r="C4" s="110" t="s">
+        <v>453</v>
+      </c>
+      <c r="D4" s="110" t="s">
+        <v>454</v>
+      </c>
+      <c r="E4" s="110" t="s">
+        <v>455</v>
+      </c>
+      <c r="F4" s="110" t="s">
+        <v>380</v>
+      </c>
+      <c r="G4" s="110" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="57" customHeight="1">
+      <c r="B5" s="104">
+        <v>1</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>479</v>
+      </c>
+      <c r="D5" s="105" t="s">
+        <v>457</v>
+      </c>
+      <c r="E5" s="106" t="s">
+        <v>390</v>
+      </c>
+      <c r="F5" s="105" t="s">
+        <v>458</v>
+      </c>
+      <c r="G5" s="105" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="54" customHeight="1">
+      <c r="B6" s="104">
+        <v>2</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>507</v>
+      </c>
+      <c r="D6" s="105" t="s">
+        <v>460</v>
+      </c>
+      <c r="E6" s="107" t="s">
+        <v>461</v>
+      </c>
+      <c r="F6" s="107" t="s">
+        <v>462</v>
+      </c>
+      <c r="G6" s="105" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="64.5" customHeight="1">
+      <c r="B7" s="111">
+        <v>3</v>
+      </c>
+      <c r="C7" s="105" t="s">
+        <v>464</v>
+      </c>
+      <c r="D7" s="105" t="s">
+        <v>465</v>
+      </c>
+      <c r="E7" s="107" t="s">
+        <v>466</v>
+      </c>
+      <c r="F7" s="105" t="s">
+        <v>467</v>
+      </c>
+      <c r="G7" s="105" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.75">
+      <c r="B10" s="114" t="s">
+        <v>482</v>
+      </c>
+      <c r="C10" s="115"/>
+      <c r="D10" s="116"/>
+    </row>
+    <row r="11" spans="2:7" ht="15.75">
+      <c r="B11" s="113" t="s">
+        <v>376</v>
+      </c>
+      <c r="C11" s="113" t="s">
+        <v>453</v>
+      </c>
+      <c r="D11" s="113" t="s">
+        <v>454</v>
+      </c>
+      <c r="E11" s="113" t="s">
+        <v>455</v>
+      </c>
+      <c r="F11" s="113" t="s">
+        <v>380</v>
+      </c>
+      <c r="G11" s="113" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="55.5" customHeight="1">
+      <c r="B12" s="67">
+        <v>1</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>470</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>457</v>
+      </c>
+      <c r="E12" s="112" t="s">
+        <v>471</v>
+      </c>
+      <c r="F12" s="68" t="s">
+        <v>405</v>
+      </c>
+      <c r="G12" s="68" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="31.5">
+      <c r="B13" s="67">
+        <v>2</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>472</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>460</v>
+      </c>
+      <c r="E13" s="70" t="s">
+        <v>473</v>
+      </c>
+      <c r="F13" s="70" t="s">
+        <v>458</v>
+      </c>
+      <c r="G13" s="68" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="44.25" customHeight="1">
+      <c r="B14" s="108">
+        <v>3</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>474</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>475</v>
+      </c>
+      <c r="E14" s="70" t="s">
+        <v>476</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>477</v>
+      </c>
+      <c r="G14" s="68" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="15.75">
+      <c r="B17" s="114" t="s">
+        <v>495</v>
+      </c>
+      <c r="C17" s="115"/>
+      <c r="D17" s="116"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.75">
+      <c r="B18" s="37" t="s">
+        <v>401</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>483</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>484</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>485</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>486</v>
+      </c>
+      <c r="G18" s="37" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="63">
+      <c r="B19" s="74">
+        <v>1</v>
+      </c>
+      <c r="C19" s="74" t="s">
+        <v>488</v>
+      </c>
+      <c r="D19" s="74" t="s">
+        <v>489</v>
+      </c>
+      <c r="E19" s="74" t="s">
+        <v>417</v>
+      </c>
+      <c r="F19" s="74" t="s">
+        <v>490</v>
+      </c>
+      <c r="G19" s="74" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="47.25">
+      <c r="B20" s="74">
+        <v>2</v>
+      </c>
+      <c r="C20" s="74" t="s">
+        <v>491</v>
+      </c>
+      <c r="D20" s="74" t="s">
+        <v>492</v>
+      </c>
+      <c r="E20" s="74" t="s">
+        <v>405</v>
+      </c>
+      <c r="F20" s="74" t="s">
+        <v>490</v>
+      </c>
+      <c r="G20" s="74" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="47.25">
+      <c r="B21" s="74">
+        <v>3</v>
+      </c>
+      <c r="C21" s="74" t="s">
+        <v>494</v>
+      </c>
+      <c r="D21" s="74" t="s">
+        <v>492</v>
+      </c>
+      <c r="E21" s="74" t="s">
+        <v>449</v>
+      </c>
+      <c r="F21" s="74" t="s">
+        <v>428</v>
+      </c>
+      <c r="G21" s="74" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="15.75">
+      <c r="B23" s="114" t="s">
+        <v>506</v>
+      </c>
+      <c r="C23" s="115"/>
+      <c r="D23" s="116"/>
+    </row>
+    <row r="24" spans="2:7" ht="15.75">
+      <c r="B24" s="37" t="s">
+        <v>401</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>483</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>484</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>485</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>486</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="47.25">
+      <c r="B25" s="74">
+        <v>1</v>
+      </c>
+      <c r="C25" s="74" t="s">
+        <v>498</v>
+      </c>
+      <c r="D25" s="74" t="s">
+        <v>489</v>
+      </c>
+      <c r="E25" s="74" t="s">
+        <v>417</v>
+      </c>
+      <c r="F25" s="74" t="s">
+        <v>428</v>
+      </c>
+      <c r="G25" s="74" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="31.5">
+      <c r="B26" s="74">
+        <v>2</v>
+      </c>
+      <c r="C26" s="74" t="s">
+        <v>500</v>
+      </c>
+      <c r="D26" s="74" t="s">
+        <v>501</v>
+      </c>
+      <c r="E26" s="74" t="s">
+        <v>449</v>
+      </c>
+      <c r="F26" s="74" t="s">
+        <v>490</v>
+      </c>
+      <c r="G26" s="74" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="31.5">
+      <c r="B27" s="74">
+        <v>3</v>
+      </c>
+      <c r="C27" s="74" t="s">
+        <v>503</v>
+      </c>
+      <c r="D27" s="74" t="s">
+        <v>504</v>
+      </c>
+      <c r="E27" s="74" t="s">
+        <v>405</v>
+      </c>
+      <c r="F27" s="74" t="s">
+        <v>471</v>
+      </c>
+      <c r="G27" s="74" t="s">
+        <v>505</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>